<commit_message>
preparation of the data in excel is almost complete
</commit_message>
<xml_diff>
--- a/North_Valley/data/North_Valley_Data.xlsx
+++ b/North_Valley/data/North_Valley_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FP\South_Valley\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FP\North_Valley\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -174,15 +174,9 @@
     <t>gips</t>
   </si>
   <si>
-    <t>г\кг</t>
-  </si>
-  <si>
     <t>мг\кг</t>
   </si>
   <si>
-    <t>мкг\кг</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -192,169 +186,61 @@
     <t>Moraine</t>
   </si>
   <si>
-    <t>347.83</t>
-  </si>
-  <si>
-    <t>1.87</t>
-  </si>
-  <si>
     <t>2012</t>
   </si>
   <si>
-    <t>213.7</t>
-  </si>
-  <si>
-    <t>0.38200000000000001</t>
-  </si>
-  <si>
     <t>2016</t>
   </si>
   <si>
     <t>Right</t>
   </si>
   <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>0.95</t>
-  </si>
-  <si>
     <t>2018</t>
   </si>
   <si>
-    <t>209.4</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.45</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
     <t>2002</t>
   </si>
   <si>
     <t>Left</t>
   </si>
   <si>
-    <t>267.74</t>
-  </si>
-  <si>
-    <t>0.76500000000000001</t>
-  </si>
-  <si>
     <t>2003</t>
   </si>
   <si>
-    <t>162.34</t>
-  </si>
-  <si>
-    <t>0.79</t>
-  </si>
-  <si>
     <t>2004</t>
   </si>
   <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>1.64</t>
-  </si>
-  <si>
     <t>2005</t>
   </si>
   <si>
-    <t>386.53</t>
-  </si>
-  <si>
-    <t>8.7999999999999995E-2</t>
-  </si>
-  <si>
     <t>2006</t>
   </si>
   <si>
-    <t>228</t>
-  </si>
-  <si>
-    <t>2.91</t>
-  </si>
-  <si>
     <t>2007</t>
   </si>
   <si>
-    <t>263.33999999999997</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
     <t>2008</t>
   </si>
   <si>
-    <t>270</t>
-  </si>
-  <si>
-    <t>0.93</t>
-  </si>
-  <si>
     <t>2009</t>
   </si>
   <si>
-    <t>246.82</t>
-  </si>
-  <si>
-    <t>0.242</t>
-  </si>
-  <si>
     <t>2011</t>
   </si>
   <si>
-    <t>268.62</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
     <t>2013</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
     <t>2014</t>
   </si>
   <si>
-    <t>277.77999999999997</t>
-  </si>
-  <si>
-    <t>1.03</t>
-  </si>
-  <si>
     <t>2017</t>
   </si>
   <si>
-    <t>364.9</t>
-  </si>
-  <si>
     <t>2015</t>
   </si>
   <si>
-    <t>155</t>
-  </si>
-  <si>
-    <t>0.17399999999999999</t>
-  </si>
-  <si>
     <t>2001</t>
-  </si>
-  <si>
-    <t>357.22</t>
-  </si>
-  <si>
-    <t>0.44</t>
   </si>
   <si>
     <t>Размерность</t>
@@ -734,7 +620,7 @@
   <dimension ref="A1:AT20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,7 +770,7 @@
     </row>
     <row r="2" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -899,126 +785,126 @@
         <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="AL2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="AM2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="AN2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="AO2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="AP2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="AR2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="AS2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="AT2" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>42.470527000320892</v>
@@ -1027,22 +913,22 @@
         <v>43.233797000131517</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3">
-        <v>1.26</v>
+        <v>1260</v>
       </c>
       <c r="F3">
-        <v>57.63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>52</v>
+        <v>57630</v>
+      </c>
+      <c r="G3">
+        <v>347830</v>
       </c>
       <c r="K3">
-        <v>32.700000000000003</v>
+        <v>32700.000000000004</v>
       </c>
       <c r="L3">
-        <v>0.64500000000000002</v>
+        <v>645</v>
       </c>
       <c r="M3">
         <v>0.68899999999999995</v>
@@ -1062,11 +948,11 @@
       <c r="S3">
         <v>0.14499999999999999</v>
       </c>
-      <c r="T3" t="s">
-        <v>53</v>
+      <c r="T3">
+        <v>1.87</v>
       </c>
       <c r="U3">
-        <v>0.27800000000000002</v>
+        <v>2.7800000000000004E-4</v>
       </c>
       <c r="V3">
         <v>0.5</v>
@@ -1078,7 +964,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="AJ3">
-        <v>0.20300000000000001</v>
+        <v>2.03E-4</v>
       </c>
       <c r="AK3">
         <v>9</v>
@@ -1113,7 +999,7 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>42.478300999991227</v>
@@ -1122,16 +1008,16 @@
         <v>43.229780000146953</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4">
-        <v>0.125</v>
+        <v>125</v>
       </c>
       <c r="F4">
-        <v>62.68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
+        <v>62680</v>
+      </c>
+      <c r="G4">
+        <v>213700</v>
       </c>
       <c r="I4">
         <v>0.5</v>
@@ -1140,10 +1026,10 @@
         <v>0.96</v>
       </c>
       <c r="K4">
-        <v>51.31</v>
+        <v>51310</v>
       </c>
       <c r="L4">
-        <v>4.7</v>
+        <v>4700</v>
       </c>
       <c r="M4">
         <v>2.74</v>
@@ -1166,11 +1052,11 @@
       <c r="S4">
         <v>0.25</v>
       </c>
-      <c r="T4" t="s">
-        <v>56</v>
+      <c r="T4">
+        <v>0.38200000000000001</v>
       </c>
       <c r="U4">
-        <v>0.26300000000000001</v>
+        <v>2.63E-4</v>
       </c>
       <c r="V4">
         <v>0.62</v>
@@ -1182,10 +1068,10 @@
         <v>1.04</v>
       </c>
       <c r="AA4">
-        <v>0.7</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="AB4">
-        <v>0.505</v>
+        <v>5.0500000000000002E-4</v>
       </c>
       <c r="AE4">
         <v>0.86</v>
@@ -1223,7 +1109,7 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <v>42.485508999640672</v>
@@ -1232,16 +1118,16 @@
         <v>43.226531999652138</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E5">
-        <v>1.02</v>
+        <v>1020</v>
       </c>
       <c r="F5">
-        <v>44.84</v>
-      </c>
-      <c r="G5" t="s">
-        <v>59</v>
+        <v>44840</v>
+      </c>
+      <c r="G5">
+        <v>130000</v>
       </c>
       <c r="H5">
         <v>2.65</v>
@@ -1253,10 +1139,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="K5">
-        <v>19.28</v>
+        <v>19280</v>
       </c>
       <c r="L5">
-        <v>8.6</v>
+        <v>8600</v>
       </c>
       <c r="M5">
         <v>4.67</v>
@@ -1270,8 +1156,8 @@
       <c r="P5">
         <v>60.4</v>
       </c>
-      <c r="T5" t="s">
-        <v>60</v>
+      <c r="T5">
+        <v>0.95</v>
       </c>
       <c r="V5">
         <v>0.77500000000000002</v>
@@ -1312,7 +1198,7 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>42.479266000425639</v>
@@ -1321,22 +1207,22 @@
         <v>43.229580999963218</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6">
-        <v>1.03</v>
+        <v>1030</v>
       </c>
       <c r="F6">
-        <v>46.91</v>
-      </c>
-      <c r="G6" t="s">
-        <v>62</v>
+        <v>46910</v>
+      </c>
+      <c r="G6">
+        <v>209400</v>
       </c>
       <c r="K6">
-        <v>20.68</v>
+        <v>20680</v>
       </c>
       <c r="L6">
-        <v>1.26</v>
+        <v>1260</v>
       </c>
       <c r="M6">
         <v>1.05</v>
@@ -1353,11 +1239,11 @@
       <c r="S6">
         <v>0.17</v>
       </c>
-      <c r="T6" t="s">
-        <v>63</v>
+      <c r="T6">
+        <v>0.5</v>
       </c>
       <c r="U6">
-        <v>2.3E-2</v>
+        <v>2.3E-5</v>
       </c>
       <c r="V6">
         <v>1.34</v>
@@ -1369,16 +1255,16 @@
         <v>1.25</v>
       </c>
       <c r="Y6">
-        <v>1.52</v>
+        <v>1.5200000000000001E-3</v>
       </c>
       <c r="AA6">
-        <v>0.44</v>
+        <v>4.4000000000000002E-4</v>
       </c>
       <c r="AC6">
-        <v>1.37</v>
+        <v>1.3700000000000001E-3</v>
       </c>
       <c r="AI6">
-        <v>1.95</v>
+        <v>1.9499999999999999E-3</v>
       </c>
       <c r="AK6">
         <v>11</v>
@@ -1413,7 +1299,7 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>42.484621000059178</v>
@@ -1422,22 +1308,22 @@
         <v>43.227588999832513</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E7">
-        <v>0.05</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>198.01499999999999</v>
-      </c>
-      <c r="G7" t="s">
-        <v>68</v>
+        <v>198015</v>
+      </c>
+      <c r="G7">
+        <v>267740</v>
       </c>
       <c r="K7">
-        <v>121.98</v>
+        <v>121980</v>
       </c>
       <c r="L7">
-        <v>7.98</v>
+        <v>7980</v>
       </c>
       <c r="M7">
         <v>23.302</v>
@@ -1457,8 +1343,8 @@
       <c r="S7">
         <v>0.54</v>
       </c>
-      <c r="T7" t="s">
-        <v>69</v>
+      <c r="T7">
+        <v>0.76500000000000001</v>
       </c>
       <c r="V7">
         <v>0.27500000000000002</v>
@@ -1467,13 +1353,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="AA7">
-        <v>3.23</v>
+        <v>3.2299999999999998E-3</v>
       </c>
       <c r="AB7">
-        <v>0.69499999999999995</v>
+        <v>6.9499999999999998E-4</v>
       </c>
       <c r="AC7">
-        <v>5.91</v>
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="AK7">
         <v>46</v>
@@ -1508,7 +1394,7 @@
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B8">
         <v>42.482531999951902</v>
@@ -1517,16 +1403,16 @@
         <v>43.228735999666704</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E8">
-        <v>1.07</v>
+        <v>1070</v>
       </c>
       <c r="F8">
-        <v>75.09</v>
-      </c>
-      <c r="G8" t="s">
-        <v>71</v>
+        <v>75090</v>
+      </c>
+      <c r="G8">
+        <v>162340</v>
       </c>
       <c r="H8">
         <v>2.5499999999999998</v>
@@ -1538,10 +1424,10 @@
         <v>1.28</v>
       </c>
       <c r="K8">
-        <v>52.64</v>
+        <v>52640</v>
       </c>
       <c r="L8">
-        <v>26.67</v>
+        <v>26670</v>
       </c>
       <c r="M8">
         <v>10.87</v>
@@ -1558,8 +1444,8 @@
       <c r="Q8">
         <v>0.19500000000000001</v>
       </c>
-      <c r="T8" t="s">
-        <v>72</v>
+      <c r="T8">
+        <v>0.79</v>
       </c>
       <c r="V8">
         <v>1.31</v>
@@ -1568,7 +1454,7 @@
         <v>3.65</v>
       </c>
       <c r="AJ8">
-        <v>0.12</v>
+        <v>1.1999999999999999E-4</v>
       </c>
       <c r="AK8">
         <v>36</v>
@@ -1603,7 +1489,7 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>42.480811999774012</v>
@@ -1612,16 +1498,16 @@
         <v>43.229299000448577</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E9">
-        <v>0.95</v>
+        <v>950</v>
       </c>
       <c r="F9">
-        <v>54.64</v>
-      </c>
-      <c r="G9" t="s">
-        <v>74</v>
+        <v>54640</v>
+      </c>
+      <c r="G9">
+        <v>330000</v>
       </c>
       <c r="H9">
         <v>0.8</v>
@@ -1633,10 +1519,10 @@
         <v>0.51</v>
       </c>
       <c r="K9">
-        <v>42.99</v>
+        <v>42990</v>
       </c>
       <c r="L9">
-        <v>7.28</v>
+        <v>7280</v>
       </c>
       <c r="M9">
         <v>6.26</v>
@@ -1656,8 +1542,8 @@
       <c r="S9">
         <v>0.47</v>
       </c>
-      <c r="T9" t="s">
-        <v>75</v>
+      <c r="T9">
+        <v>1.64</v>
       </c>
       <c r="V9">
         <v>0.65</v>
@@ -1666,10 +1552,10 @@
         <v>1.79</v>
       </c>
       <c r="AA9">
-        <v>0.95</v>
+        <v>9.5E-4</v>
       </c>
       <c r="AD9">
-        <v>0.94499999999999995</v>
+        <v>9.4499999999999998E-4</v>
       </c>
       <c r="AK9">
         <v>11</v>
@@ -1704,7 +1590,7 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>42.480762000166237</v>
@@ -1713,22 +1599,22 @@
         <v>43.229126999711298</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E10">
-        <v>3.26</v>
+        <v>3260</v>
       </c>
       <c r="F10">
-        <v>15.89</v>
-      </c>
-      <c r="G10" t="s">
-        <v>77</v>
+        <v>15890</v>
+      </c>
+      <c r="G10">
+        <v>386530</v>
       </c>
       <c r="K10">
-        <v>5.92</v>
+        <v>5920</v>
       </c>
       <c r="L10">
-        <v>0.42</v>
+        <v>420</v>
       </c>
       <c r="M10">
         <v>0.47</v>
@@ -1745,11 +1631,11 @@
       <c r="S10">
         <v>0.1</v>
       </c>
-      <c r="T10" t="s">
-        <v>78</v>
+      <c r="T10">
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="U10">
-        <v>0.41799999999999998</v>
+        <v>4.1799999999999997E-4</v>
       </c>
       <c r="V10">
         <v>0.32</v>
@@ -1761,7 +1647,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="AA10">
-        <v>0.38</v>
+        <v>3.8000000000000002E-4</v>
       </c>
       <c r="AK10">
         <v>12</v>
@@ -1796,7 +1682,7 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>42.479376000102377</v>
@@ -1805,22 +1691,22 @@
         <v>43.229760000123967</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E11">
-        <v>0.24</v>
+        <v>240</v>
       </c>
       <c r="F11">
-        <v>138.05000000000001</v>
-      </c>
-      <c r="G11" t="s">
-        <v>80</v>
+        <v>138050</v>
+      </c>
+      <c r="G11">
+        <v>228000</v>
       </c>
       <c r="K11">
-        <v>54.33</v>
+        <v>54330</v>
       </c>
       <c r="L11">
-        <v>3.45</v>
+        <v>3450</v>
       </c>
       <c r="M11">
         <v>3.12</v>
@@ -1834,8 +1720,8 @@
       <c r="S11">
         <v>1.375</v>
       </c>
-      <c r="T11" t="s">
-        <v>81</v>
+      <c r="T11">
+        <v>2.91</v>
       </c>
       <c r="V11">
         <v>0.82</v>
@@ -1844,7 +1730,7 @@
         <v>1.835</v>
       </c>
       <c r="AA11">
-        <v>0.32800000000000001</v>
+        <v>3.28E-4</v>
       </c>
       <c r="AK11">
         <v>18</v>
@@ -1879,7 +1765,7 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>42.477304999925877</v>
@@ -1888,25 +1774,25 @@
         <v>43.230735000120212</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E12">
-        <v>4.62</v>
+        <v>4620</v>
       </c>
       <c r="F12">
-        <v>65.48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>83</v>
+        <v>65480.000000000007</v>
+      </c>
+      <c r="G12">
+        <v>263339.99999999901</v>
       </c>
       <c r="I12">
         <v>1.07</v>
       </c>
       <c r="K12">
-        <v>14.39</v>
+        <v>14390</v>
       </c>
       <c r="L12">
-        <v>9.23</v>
+        <v>9230</v>
       </c>
       <c r="M12">
         <v>9.7000000000000003E-2</v>
@@ -1929,11 +1815,11 @@
       <c r="S12">
         <v>0.36</v>
       </c>
-      <c r="T12" t="s">
-        <v>84</v>
+      <c r="T12">
+        <v>0.25</v>
       </c>
       <c r="U12">
-        <v>5.1999999999999998E-2</v>
+        <v>5.1999999999999997E-5</v>
       </c>
       <c r="V12">
         <v>0.61</v>
@@ -1948,7 +1834,7 @@
         <v>2.21</v>
       </c>
       <c r="AF12">
-        <v>0.96299999999999997</v>
+        <v>9.6299999999999999E-4</v>
       </c>
       <c r="AK12">
         <v>10</v>
@@ -1983,7 +1869,7 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B13">
         <v>42.476786000273762</v>
@@ -1992,25 +1878,25 @@
         <v>43.231610000001517</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E13">
-        <v>14.27</v>
+        <v>14270</v>
       </c>
       <c r="F13">
-        <v>104.97</v>
-      </c>
-      <c r="G13" t="s">
-        <v>86</v>
+        <v>104970</v>
+      </c>
+      <c r="G13">
+        <v>270000</v>
       </c>
       <c r="J13">
         <v>1.1499999999999999</v>
       </c>
       <c r="K13">
-        <v>53.05</v>
+        <v>53050</v>
       </c>
       <c r="L13">
-        <v>7.69</v>
+        <v>7690</v>
       </c>
       <c r="M13">
         <v>6.14</v>
@@ -2033,11 +1919,11 @@
       <c r="S13">
         <v>0.97</v>
       </c>
-      <c r="T13" t="s">
-        <v>87</v>
+      <c r="T13">
+        <v>0.93</v>
       </c>
       <c r="U13">
-        <v>0.11</v>
+        <v>1.1E-4</v>
       </c>
       <c r="V13">
         <v>0.62</v>
@@ -2081,7 +1967,7 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>42.474755000143212</v>
@@ -2090,22 +1976,22 @@
         <v>43.232109999676823</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E14">
-        <v>8.3000000000000004E-2</v>
+        <v>83</v>
       </c>
       <c r="F14">
-        <v>181.98</v>
-      </c>
-      <c r="G14" t="s">
-        <v>89</v>
+        <v>181980</v>
+      </c>
+      <c r="G14">
+        <v>246820</v>
       </c>
       <c r="K14">
-        <v>121.44</v>
+        <v>121440</v>
       </c>
       <c r="L14">
-        <v>0.89</v>
+        <v>890</v>
       </c>
       <c r="M14">
         <v>6.12</v>
@@ -2128,8 +2014,8 @@
       <c r="S14">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="T14" t="s">
-        <v>90</v>
+      <c r="T14">
+        <v>0.24199999999999999</v>
       </c>
       <c r="V14">
         <v>0.53300000000000003</v>
@@ -2170,7 +2056,7 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="B15">
         <v>42.477310000156422</v>
@@ -2179,22 +2065,22 @@
         <v>43.229892999962033</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E15">
-        <v>0.37</v>
+        <v>370</v>
       </c>
       <c r="F15">
-        <v>111.09</v>
-      </c>
-      <c r="G15" t="s">
-        <v>92</v>
+        <v>111090</v>
+      </c>
+      <c r="G15">
+        <v>268620</v>
       </c>
       <c r="K15">
-        <v>75.540000000000006</v>
+        <v>75540</v>
       </c>
       <c r="L15">
-        <v>6.97</v>
+        <v>6970</v>
       </c>
       <c r="M15">
         <v>7.0990000000000002</v>
@@ -2211,8 +2097,8 @@
       <c r="S15">
         <v>0.53</v>
       </c>
-      <c r="T15" t="s">
-        <v>93</v>
+      <c r="T15">
+        <v>0.82</v>
       </c>
       <c r="V15">
         <v>0.76</v>
@@ -2253,7 +2139,7 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B16">
         <v>42.479828000262053</v>
@@ -2262,16 +2148,16 @@
         <v>43.229155000103219</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E16">
-        <v>0.26</v>
+        <v>260</v>
       </c>
       <c r="F16">
-        <v>74.105000000000004</v>
-      </c>
-      <c r="G16" t="s">
-        <v>95</v>
+        <v>74105</v>
+      </c>
+      <c r="G16">
+        <v>300000</v>
       </c>
       <c r="H16">
         <v>0.4</v>
@@ -2283,10 +2169,10 @@
         <v>1.075</v>
       </c>
       <c r="K16">
-        <v>24.22</v>
+        <v>24220</v>
       </c>
       <c r="L16">
-        <v>3.21</v>
+        <v>3210</v>
       </c>
       <c r="M16">
         <v>0.57299999999999995</v>
@@ -2309,8 +2195,8 @@
       <c r="S16">
         <v>0.25</v>
       </c>
-      <c r="T16" t="s">
-        <v>65</v>
+      <c r="T16">
+        <v>0.22</v>
       </c>
       <c r="V16">
         <v>0.52</v>
@@ -2319,10 +2205,10 @@
         <v>0.91</v>
       </c>
       <c r="AA16">
-        <v>0.54</v>
+        <v>5.4000000000000001E-4</v>
       </c>
       <c r="AG16">
-        <v>2.63</v>
+        <v>2.63E-3</v>
       </c>
       <c r="AK16">
         <v>10</v>
@@ -2357,7 +2243,7 @@
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B17">
         <v>42.482537000182447</v>
@@ -2366,22 +2252,22 @@
         <v>43.228182000199183</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E17">
-        <v>0.23</v>
+        <v>230</v>
       </c>
       <c r="F17">
-        <v>102.15</v>
-      </c>
-      <c r="G17" t="s">
-        <v>97</v>
+        <v>102150</v>
+      </c>
+      <c r="G17">
+        <v>277779.99999999901</v>
       </c>
       <c r="K17">
-        <v>184.33</v>
+        <v>184330</v>
       </c>
       <c r="L17">
-        <v>4.62</v>
+        <v>4620</v>
       </c>
       <c r="M17">
         <v>4.82</v>
@@ -2398,8 +2284,8 @@
       <c r="S17">
         <v>0.33</v>
       </c>
-      <c r="T17" t="s">
-        <v>98</v>
+      <c r="T17">
+        <v>1.03</v>
       </c>
       <c r="V17">
         <v>0.67</v>
@@ -2408,7 +2294,7 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="AA17">
-        <v>1.07</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AK17">
         <v>29</v>
@@ -2443,7 +2329,7 @@
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B18">
         <v>42.480339000444587</v>
@@ -2452,16 +2338,16 @@
         <v>43.229045000426481</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E18">
-        <v>20.54</v>
+        <v>20540</v>
       </c>
       <c r="F18">
-        <v>129.5</v>
-      </c>
-      <c r="G18" t="s">
-        <v>100</v>
+        <v>129500</v>
+      </c>
+      <c r="G18">
+        <v>364900</v>
       </c>
       <c r="I18">
         <v>0.47</v>
@@ -2470,10 +2356,10 @@
         <v>0.96</v>
       </c>
       <c r="K18">
-        <v>89.9</v>
+        <v>89900</v>
       </c>
       <c r="L18">
-        <v>7.72</v>
+        <v>7720</v>
       </c>
       <c r="M18">
         <v>12.44</v>
@@ -2490,8 +2376,8 @@
       <c r="S18">
         <v>0.55000000000000004</v>
       </c>
-      <c r="T18" t="s">
-        <v>64</v>
+      <c r="T18">
+        <v>0.45</v>
       </c>
       <c r="V18">
         <v>1.05</v>
@@ -2500,7 +2386,7 @@
         <v>3.81</v>
       </c>
       <c r="AD18">
-        <v>1.6240000000000001</v>
+        <v>1.624E-3</v>
       </c>
       <c r="AK18">
         <v>15</v>
@@ -2535,7 +2421,7 @@
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B19">
         <v>42.485105309262678</v>
@@ -2544,22 +2430,22 @@
         <v>43.227299262550957</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19">
-        <v>0.05</v>
+        <v>50</v>
       </c>
       <c r="F19">
-        <v>11.28</v>
-      </c>
-      <c r="G19" t="s">
-        <v>102</v>
+        <v>11280</v>
+      </c>
+      <c r="G19">
+        <v>155000</v>
       </c>
       <c r="K19">
-        <v>5.65</v>
+        <v>5650</v>
       </c>
       <c r="L19">
-        <v>0.57999999999999996</v>
+        <v>580</v>
       </c>
       <c r="M19">
         <v>0.34</v>
@@ -2579,8 +2465,8 @@
       <c r="S19">
         <v>0.16300000000000001</v>
       </c>
-      <c r="T19" t="s">
-        <v>103</v>
+      <c r="T19">
+        <v>0.17399999999999899</v>
       </c>
       <c r="V19">
         <v>0.56000000000000005</v>
@@ -2589,7 +2475,7 @@
         <v>0.17</v>
       </c>
       <c r="AD19">
-        <v>0.68</v>
+        <v>6.8000000000000005E-4</v>
       </c>
       <c r="AK19">
         <v>4</v>
@@ -2624,7 +2510,7 @@
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B20">
         <v>42.486509999936573</v>
@@ -2633,25 +2519,25 @@
         <v>43.228030000384251</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E20">
-        <v>4.1040000000000001</v>
+        <v>4104</v>
       </c>
       <c r="F20">
-        <v>60.853999999999999</v>
-      </c>
-      <c r="G20" t="s">
-        <v>105</v>
+        <v>60854</v>
+      </c>
+      <c r="G20">
+        <v>357220</v>
       </c>
       <c r="I20">
         <v>0.23</v>
       </c>
       <c r="K20">
-        <v>54.93</v>
+        <v>54930</v>
       </c>
       <c r="L20">
-        <v>1.33</v>
+        <v>1330</v>
       </c>
       <c r="M20">
         <v>3.71</v>
@@ -2665,11 +2551,11 @@
       <c r="S20">
         <v>0.25700000000000001</v>
       </c>
-      <c r="T20" t="s">
-        <v>106</v>
+      <c r="T20">
+        <v>0.44</v>
       </c>
       <c r="U20">
-        <v>0.35</v>
+        <v>3.5E-4</v>
       </c>
       <c r="V20">
         <v>0.21</v>
@@ -2681,10 +2567,10 @@
         <v>1.34</v>
       </c>
       <c r="Y20">
-        <v>1.48</v>
+        <v>1.48E-3</v>
       </c>
       <c r="Z20">
-        <v>1.91</v>
+        <v>1.91E-3</v>
       </c>
       <c r="AK20">
         <v>32</v>
@@ -2719,5 +2605,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data reading is complete
</commit_message>
<xml_diff>
--- a/North_Valley/data/North_Valley_Data.xlsx
+++ b/North_Valley/data/North_Valley_Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -180,77 +180,29 @@
     <t>%</t>
   </si>
   <si>
-    <t>2010</t>
-  </si>
-  <si>
     <t>Moraine</t>
   </si>
   <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
     <t>Right</t>
   </si>
   <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
     <t>Left</t>
   </si>
   <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2008</t>
-  </si>
-  <si>
-    <t>2009</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
     <t>Размерность</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Mix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +222,15 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -297,12 +258,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -617,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT20"/>
+  <dimension ref="A1:AT22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,7 +732,7 @@
     </row>
     <row r="2" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -903,8 +865,8 @@
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>48</v>
+      <c r="A3">
+        <v>2010</v>
       </c>
       <c r="B3">
         <v>42.470527000320892</v>
@@ -913,7 +875,7 @@
         <v>43.233797000131517</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>1260</v>
@@ -998,8 +960,8 @@
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>50</v>
+      <c r="A4">
+        <v>2012</v>
       </c>
       <c r="B4">
         <v>42.478300999991227</v>
@@ -1008,7 +970,7 @@
         <v>43.229780000146953</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>125</v>
@@ -1108,8 +1070,8 @@
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>51</v>
+      <c r="A5">
+        <v>2016</v>
       </c>
       <c r="B5">
         <v>42.485508999640672</v>
@@ -1118,7 +1080,7 @@
         <v>43.226531999652138</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>1020</v>
@@ -1197,8 +1159,8 @@
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>53</v>
+      <c r="A6">
+        <v>2018</v>
       </c>
       <c r="B6">
         <v>42.479266000425639</v>
@@ -1207,7 +1169,7 @@
         <v>43.229580999963218</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>1030</v>
@@ -1298,8 +1260,8 @@
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>54</v>
+      <c r="A7">
+        <v>2002</v>
       </c>
       <c r="B7">
         <v>42.484621000059178</v>
@@ -1308,7 +1270,7 @@
         <v>43.227588999832513</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -1393,8 +1355,8 @@
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>56</v>
+      <c r="A8">
+        <v>2003</v>
       </c>
       <c r="B8">
         <v>42.482531999951902</v>
@@ -1403,7 +1365,7 @@
         <v>43.228735999666704</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>1070</v>
@@ -1488,8 +1450,8 @@
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>57</v>
+      <c r="A9">
+        <v>2004</v>
       </c>
       <c r="B9">
         <v>42.480811999774012</v>
@@ -1498,7 +1460,7 @@
         <v>43.229299000448577</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>950</v>
@@ -1589,8 +1551,8 @@
       </c>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>58</v>
+      <c r="A10">
+        <v>2005</v>
       </c>
       <c r="B10">
         <v>42.480762000166237</v>
@@ -1599,7 +1561,7 @@
         <v>43.229126999711298</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E10">
         <v>3260</v>
@@ -1681,8 +1643,8 @@
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>59</v>
+      <c r="A11">
+        <v>2006</v>
       </c>
       <c r="B11">
         <v>42.479376000102377</v>
@@ -1691,7 +1653,7 @@
         <v>43.229760000123967</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E11">
         <v>240</v>
@@ -1764,8 +1726,8 @@
       </c>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>60</v>
+      <c r="A12">
+        <v>2007</v>
       </c>
       <c r="B12">
         <v>42.477304999925877</v>
@@ -1774,7 +1736,7 @@
         <v>43.230735000120212</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>4620</v>
@@ -1868,8 +1830,8 @@
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>61</v>
+      <c r="A13">
+        <v>2008</v>
       </c>
       <c r="B13">
         <v>42.476786000273762</v>
@@ -1878,7 +1840,7 @@
         <v>43.231610000001517</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13">
         <v>14270</v>
@@ -1966,8 +1928,8 @@
       </c>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>62</v>
+      <c r="A14">
+        <v>2009</v>
       </c>
       <c r="B14">
         <v>42.474755000143212</v>
@@ -1976,7 +1938,7 @@
         <v>43.232109999676823</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>83</v>
@@ -2055,8 +2017,8 @@
       </c>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>63</v>
+      <c r="A15">
+        <v>2011</v>
       </c>
       <c r="B15">
         <v>42.477310000156422</v>
@@ -2065,7 +2027,7 @@
         <v>43.229892999962033</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15">
         <v>370</v>
@@ -2138,8 +2100,8 @@
       </c>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>64</v>
+      <c r="A16">
+        <v>2013</v>
       </c>
       <c r="B16">
         <v>42.479828000262053</v>
@@ -2148,7 +2110,7 @@
         <v>43.229155000103219</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16">
         <v>260</v>
@@ -2242,8 +2204,8 @@
       </c>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>65</v>
+      <c r="A17">
+        <v>2014</v>
       </c>
       <c r="B17">
         <v>42.482537000182447</v>
@@ -2252,7 +2214,7 @@
         <v>43.228182000199183</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E17">
         <v>230</v>
@@ -2328,8 +2290,8 @@
       </c>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>66</v>
+      <c r="A18">
+        <v>2017</v>
       </c>
       <c r="B18">
         <v>42.480339000444587</v>
@@ -2338,7 +2300,7 @@
         <v>43.229045000426481</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18">
         <v>20540</v>
@@ -2420,8 +2382,8 @@
       </c>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>67</v>
+      <c r="A19">
+        <v>2015</v>
       </c>
       <c r="B19">
         <v>42.485105309262678</v>
@@ -2430,7 +2392,7 @@
         <v>43.227299262550957</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19">
         <v>50</v>
@@ -2509,8 +2471,8 @@
       </c>
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>68</v>
+      <c r="A20">
+        <v>2001</v>
       </c>
       <c r="B20">
         <v>42.486509999936573</v>
@@ -2519,7 +2481,7 @@
         <v>43.228030000384251</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E20">
         <v>4104</v>
@@ -2602,6 +2564,99 @@
       <c r="AT20">
         <v>0</v>
       </c>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>3000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>5.03</v>
+      </c>
+      <c r="G21" s="3">
+        <v>427.3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
+        <v>3.68</v>
+      </c>
+      <c r="L21" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="P21" s="3">
+        <v>12.35</v>
+      </c>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="W21" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AK21" s="3">
+        <v>9</v>
+      </c>
+      <c r="AL21" s="3"/>
+      <c r="AM21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP21" s="3">
+        <v>59</v>
+      </c>
+      <c r="AQ21" s="3">
+        <v>13</v>
+      </c>
+      <c r="AR21" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
+      <c r="AP22" s="3"/>
+      <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
need to check points
</commit_message>
<xml_diff>
--- a/North_Valley/data/North_Valley_Data.xlsx
+++ b/North_Valley/data/North_Valley_Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>Размерность</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>Mix</t>
@@ -581,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2570,14 +2567,16 @@
         <v>3000</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3">
-        <v>5.03</v>
+        <f>5.03*1000</f>
+        <v>5030</v>
       </c>
       <c r="G21" s="3">
-        <v>427.3</v>
+        <f>427.3*1000</f>
+        <v>427300</v>
       </c>
       <c r="H21" s="3">
         <v>0.9</v>
@@ -2585,17 +2584,20 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3">
-        <v>3.68</v>
+        <f>3.68*1000</f>
+        <v>3680</v>
       </c>
       <c r="L21" s="3">
-        <v>2.9</v>
+        <f>2.9*1000</f>
+        <v>2900</v>
       </c>
       <c r="M21" s="3">
         <v>0.81</v>
       </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3">
-        <v>2.1</v>
+        <f>2.1/1000</f>
+        <v>2.1000000000000003E-3</v>
       </c>
       <c r="P21" s="3">
         <v>12.35</v>
@@ -2617,8 +2619,8 @@
         <v>9</v>
       </c>
       <c r="AL21" s="3"/>
-      <c r="AM21" s="3" t="s">
-        <v>52</v>
+      <c r="AM21" s="3">
+        <v>2</v>
       </c>
       <c r="AP21" s="3">
         <v>59</v>

</xml_diff>

<commit_message>
in progress but too few moraine points
</commit_message>
<xml_diff>
--- a/North_Valley/data/North_Valley_Data.xlsx
+++ b/North_Valley/data/North_Valley_Data.xlsx
@@ -1,40 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FP\North_Valley\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -174,25 +159,25 @@
     <t>gips</t>
   </si>
   <si>
+    <t>Размерность</t>
+  </si>
+  <si>
     <t>мг\кг</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
     <t>Moraine</t>
-  </si>
-  <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>Left</t>
-  </si>
-  <si>
-    <t>Размерность</t>
-  </si>
-  <si>
-    <t>Mix</t>
   </si>
 </sst>
 </file>
@@ -201,6 +186,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -219,15 +212,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -257,11 +241,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -296,7 +280,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -308,7 +292,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -355,23 +339,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -407,23 +374,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -576,16 +526,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT22"/>
+  <dimension ref="A1:AT17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -729,210 +676,204 @@
     </row>
     <row r="2" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="B3">
-        <v>42.470527000320892</v>
+        <v>42.485508999640672</v>
       </c>
       <c r="C3">
-        <v>43.233797000131517</v>
+        <v>43.226531999652138</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E3">
-        <v>1260</v>
+        <v>1020</v>
       </c>
       <c r="F3">
-        <v>57630</v>
+        <v>44840</v>
       </c>
       <c r="G3">
-        <v>347830</v>
+        <v>130000</v>
+      </c>
+      <c r="H3">
+        <v>2.65</v>
+      </c>
+      <c r="I3">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="J3">
+        <v>1.1599999999999999</v>
       </c>
       <c r="K3">
-        <v>32700.000000000004</v>
+        <v>19280</v>
       </c>
       <c r="L3">
-        <v>645</v>
+        <v>8600</v>
       </c>
       <c r="M3">
-        <v>0.68899999999999995</v>
+        <v>4.67</v>
+      </c>
+      <c r="N3">
+        <v>0.128</v>
       </c>
       <c r="O3">
-        <v>0.71</v>
+        <v>1.52</v>
       </c>
       <c r="P3">
-        <v>7.38</v>
-      </c>
-      <c r="Q3">
-        <v>0.62</v>
-      </c>
-      <c r="R3">
-        <v>0.106</v>
-      </c>
-      <c r="S3">
-        <v>0.14499999999999999</v>
+        <v>60.4</v>
       </c>
       <c r="T3">
-        <v>1.87</v>
-      </c>
-      <c r="U3">
-        <v>2.7800000000000004E-4</v>
+        <v>0.95</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="W3">
-        <v>0.311</v>
-      </c>
-      <c r="X3">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="AJ3">
-        <v>2.03E-4</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="AK3">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AL3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AN3">
         <v>0</v>
@@ -941,13 +882,13 @@
         <v>0</v>
       </c>
       <c r="AP3">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="AQ3">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="AR3">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="AS3">
         <v>0</v>
@@ -958,103 +899,88 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2012</v>
+        <v>2002</v>
       </c>
       <c r="B4">
-        <v>42.478300999991227</v>
+        <v>42.484621000059178</v>
       </c>
       <c r="C4">
-        <v>43.229780000146953</v>
+        <v>43.227588999832513</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E4">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="F4">
-        <v>62680</v>
+        <v>198015</v>
       </c>
       <c r="G4">
-        <v>213700</v>
-      </c>
-      <c r="I4">
-        <v>0.5</v>
-      </c>
-      <c r="J4">
-        <v>0.96</v>
+        <v>267740</v>
       </c>
       <c r="K4">
-        <v>51310</v>
+        <v>121980</v>
       </c>
       <c r="L4">
-        <v>4700</v>
+        <v>7980</v>
       </c>
       <c r="M4">
-        <v>2.74</v>
+        <v>23.302</v>
       </c>
       <c r="N4">
-        <v>7.4999999999999997E-2</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="O4">
-        <v>0.63500000000000001</v>
+        <v>3.39</v>
       </c>
       <c r="P4">
-        <v>41.65</v>
-      </c>
-      <c r="Q4">
-        <v>0.73</v>
+        <v>369.84</v>
       </c>
       <c r="R4">
-        <v>0.13500000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="S4">
-        <v>0.25</v>
+        <v>0.54</v>
       </c>
       <c r="T4">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="U4">
-        <v>2.63E-4</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="V4">
-        <v>0.62</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="W4">
-        <v>1.67</v>
-      </c>
-      <c r="X4">
-        <v>1.04</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="AA4">
-        <v>6.9999999999999999E-4</v>
+        <v>3.2299999999999998E-3</v>
       </c>
       <c r="AB4">
-        <v>5.0500000000000002E-4</v>
-      </c>
-      <c r="AE4">
-        <v>0.86</v>
+        <v>6.9499999999999998E-4</v>
+      </c>
+      <c r="AC4">
+        <v>5.9100000000000003E-3</v>
       </c>
       <c r="AK4">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="AL4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AM4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AN4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AO4">
         <v>0</v>
       </c>
       <c r="AP4">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="AQ4">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="AR4">
         <v>13</v>
@@ -1068,67 +994,73 @@
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="B5">
-        <v>42.485508999640672</v>
+        <v>42.482531999951902</v>
       </c>
       <c r="C5">
-        <v>43.226531999652138</v>
+        <v>43.228735999666704</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5">
-        <v>1020</v>
+        <v>1070</v>
       </c>
       <c r="F5">
-        <v>44840</v>
+        <v>75090</v>
       </c>
       <c r="G5">
-        <v>130000</v>
+        <v>162340</v>
       </c>
       <c r="H5">
-        <v>2.65</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="I5">
-        <v>2.4300000000000002</v>
+        <v>5.23</v>
       </c>
       <c r="J5">
-        <v>1.1599999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="K5">
-        <v>19280</v>
+        <v>52640</v>
       </c>
       <c r="L5">
-        <v>8600</v>
+        <v>26670</v>
       </c>
       <c r="M5">
-        <v>4.67</v>
+        <v>10.87</v>
       </c>
       <c r="N5">
-        <v>0.128</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="O5">
-        <v>1.52</v>
+        <v>2.95</v>
       </c>
       <c r="P5">
-        <v>60.4</v>
+        <v>111.05</v>
+      </c>
+      <c r="Q5">
+        <v>0.19500000000000001</v>
       </c>
       <c r="T5">
-        <v>0.95</v>
+        <v>0.79</v>
       </c>
       <c r="V5">
-        <v>0.77500000000000002</v>
+        <v>1.31</v>
       </c>
       <c r="W5">
-        <v>0.83399999999999996</v>
+        <v>3.65</v>
+      </c>
+      <c r="AJ5">
+        <v>1.1999999999999999E-4</v>
       </c>
       <c r="AK5">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="AL5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM5">
         <v>3</v>
@@ -1140,13 +1072,13 @@
         <v>0</v>
       </c>
       <c r="AP5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AQ5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR5">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="AS5">
         <v>0</v>
@@ -1157,79 +1089,79 @@
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2018</v>
+        <v>2004</v>
       </c>
       <c r="B6">
-        <v>42.479266000425639</v>
+        <v>42.480811999774012</v>
       </c>
       <c r="C6">
-        <v>43.229580999963218</v>
+        <v>43.229299000448577</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>1030</v>
+        <v>950</v>
       </c>
       <c r="F6">
-        <v>46910</v>
+        <v>54640</v>
       </c>
       <c r="G6">
-        <v>209400</v>
+        <v>330000</v>
+      </c>
+      <c r="H6">
+        <v>0.8</v>
+      </c>
+      <c r="I6">
+        <v>1.22</v>
+      </c>
+      <c r="J6">
+        <v>0.51</v>
       </c>
       <c r="K6">
-        <v>20680</v>
+        <v>42990</v>
       </c>
       <c r="L6">
-        <v>1260</v>
+        <v>7280</v>
       </c>
       <c r="M6">
-        <v>1.05</v>
+        <v>6.26</v>
       </c>
       <c r="O6">
-        <v>0.85</v>
+        <v>1.47</v>
       </c>
       <c r="P6">
-        <v>12.41</v>
+        <v>82.4</v>
       </c>
       <c r="Q6">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="R6">
+        <v>0.23</v>
+      </c>
+      <c r="S6">
         <v>0.47</v>
       </c>
-      <c r="S6">
-        <v>0.17</v>
-      </c>
       <c r="T6">
-        <v>0.5</v>
-      </c>
-      <c r="U6">
-        <v>2.3E-5</v>
+        <v>1.64</v>
       </c>
       <c r="V6">
-        <v>1.34</v>
+        <v>0.65</v>
       </c>
       <c r="W6">
-        <v>0.18</v>
-      </c>
-      <c r="X6">
-        <v>1.25</v>
-      </c>
-      <c r="Y6">
-        <v>1.5200000000000001E-3</v>
+        <v>1.79</v>
       </c>
       <c r="AA6">
-        <v>4.4000000000000002E-4</v>
-      </c>
-      <c r="AC6">
-        <v>1.3700000000000001E-3</v>
-      </c>
-      <c r="AI6">
-        <v>1.9499999999999999E-3</v>
+        <v>9.5E-4</v>
+      </c>
+      <c r="AD6">
+        <v>9.4499999999999998E-4</v>
       </c>
       <c r="AK6">
         <v>11</v>
       </c>
       <c r="AL6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM6">
         <v>2</v>
@@ -1241,13 +1173,13 @@
         <v>0</v>
       </c>
       <c r="AP6">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="AQ6">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AR6">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AS6">
         <v>0</v>
@@ -1258,91 +1190,94 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2002</v>
+        <v>2008</v>
       </c>
       <c r="B7">
-        <v>42.484621000059178</v>
+        <v>42.476786000273762</v>
       </c>
       <c r="C7">
-        <v>43.227588999832513</v>
+        <v>43.231610000001517</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>14270</v>
       </c>
       <c r="F7">
-        <v>198015</v>
+        <v>104970</v>
       </c>
       <c r="G7">
-        <v>267740</v>
+        <v>270000</v>
+      </c>
+      <c r="J7">
+        <v>1.1499999999999999</v>
       </c>
       <c r="K7">
-        <v>121980</v>
+        <v>53050</v>
       </c>
       <c r="L7">
-        <v>7980</v>
+        <v>7690</v>
       </c>
       <c r="M7">
-        <v>23.302</v>
+        <v>6.14</v>
       </c>
       <c r="N7">
-        <v>1.1399999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="O7">
-        <v>3.39</v>
+        <v>2.12</v>
       </c>
       <c r="P7">
-        <v>369.84</v>
+        <v>84.26</v>
+      </c>
+      <c r="Q7">
+        <v>1.68</v>
       </c>
       <c r="R7">
-        <v>0.15</v>
+        <v>0.36</v>
       </c>
       <c r="S7">
-        <v>0.54</v>
+        <v>0.97</v>
       </c>
       <c r="T7">
-        <v>0.76500000000000001</v>
+        <v>0.93</v>
+      </c>
+      <c r="U7">
+        <v>1.1E-4</v>
       </c>
       <c r="V7">
-        <v>0.27500000000000002</v>
+        <v>0.62</v>
       </c>
       <c r="W7">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="AA7">
-        <v>3.2299999999999998E-3</v>
-      </c>
-      <c r="AB7">
-        <v>6.9499999999999998E-4</v>
-      </c>
-      <c r="AC7">
-        <v>5.9100000000000003E-3</v>
+        <v>4.1639999999999997</v>
+      </c>
+      <c r="X7">
+        <v>0.998</v>
       </c>
       <c r="AK7">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="AL7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AN7">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AO7">
         <v>0</v>
       </c>
       <c r="AP7">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="AQ7">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="AR7">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AS7">
         <v>0</v>
@@ -1353,91 +1288,85 @@
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2003</v>
+        <v>2009</v>
       </c>
       <c r="B8">
-        <v>42.482531999951902</v>
+        <v>42.474755000143212</v>
       </c>
       <c r="C8">
-        <v>43.228735999666704</v>
+        <v>43.232109999676823</v>
       </c>
       <c r="D8" t="s">
         <v>50</v>
       </c>
       <c r="E8">
-        <v>1070</v>
+        <v>83</v>
       </c>
       <c r="F8">
-        <v>75090</v>
+        <v>181980</v>
       </c>
       <c r="G8">
-        <v>162340</v>
-      </c>
-      <c r="H8">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="I8">
-        <v>5.23</v>
-      </c>
-      <c r="J8">
-        <v>1.28</v>
+        <v>246820</v>
       </c>
       <c r="K8">
-        <v>52640</v>
+        <v>121440</v>
       </c>
       <c r="L8">
-        <v>26670</v>
+        <v>890</v>
       </c>
       <c r="M8">
-        <v>10.87</v>
+        <v>6.12</v>
       </c>
       <c r="N8">
-        <v>0.28000000000000003</v>
+        <v>0.435</v>
       </c>
       <c r="O8">
-        <v>2.95</v>
+        <v>0.84</v>
       </c>
       <c r="P8">
-        <v>111.05</v>
+        <v>67.7</v>
       </c>
       <c r="Q8">
-        <v>0.19500000000000001</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R8">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="S8">
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="T8">
-        <v>0.79</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="V8">
-        <v>1.31</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="W8">
-        <v>3.65</v>
-      </c>
-      <c r="AJ8">
-        <v>1.1999999999999999E-4</v>
+        <v>3.8</v>
       </c>
       <c r="AK8">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="AL8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AM8">
         <v>3</v>
       </c>
       <c r="AN8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AO8">
         <v>0</v>
       </c>
       <c r="AP8">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="AQ8">
         <v>2</v>
       </c>
       <c r="AR8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AS8">
         <v>0</v>
@@ -1448,82 +1377,64 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="B9">
-        <v>42.480811999774012</v>
+        <v>42.477310000156422</v>
       </c>
       <c r="C9">
-        <v>43.229299000448577</v>
+        <v>43.229892999962033</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9">
-        <v>950</v>
+        <v>370</v>
       </c>
       <c r="F9">
-        <v>54640</v>
+        <v>111090</v>
       </c>
       <c r="G9">
-        <v>330000</v>
-      </c>
-      <c r="H9">
-        <v>0.8</v>
-      </c>
-      <c r="I9">
-        <v>1.22</v>
-      </c>
-      <c r="J9">
-        <v>0.51</v>
+        <v>268620</v>
       </c>
       <c r="K9">
-        <v>42990</v>
+        <v>75540</v>
       </c>
       <c r="L9">
-        <v>7280</v>
+        <v>6970</v>
       </c>
       <c r="M9">
-        <v>6.26</v>
+        <v>7.0990000000000002</v>
+      </c>
+      <c r="N9">
+        <v>0.62</v>
       </c>
       <c r="O9">
-        <v>1.47</v>
+        <v>1.37</v>
       </c>
       <c r="P9">
-        <v>82.4</v>
-      </c>
-      <c r="Q9">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="R9">
-        <v>0.23</v>
+        <v>92.25</v>
       </c>
       <c r="S9">
-        <v>0.47</v>
+        <v>0.53</v>
       </c>
       <c r="T9">
-        <v>1.64</v>
+        <v>0.82</v>
       </c>
       <c r="V9">
-        <v>0.65</v>
+        <v>0.76</v>
       </c>
       <c r="W9">
-        <v>1.79</v>
-      </c>
-      <c r="AA9">
-        <v>9.5E-4</v>
-      </c>
-      <c r="AD9">
-        <v>9.4499999999999998E-4</v>
+        <v>3.25</v>
       </c>
       <c r="AK9">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="AL9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AM9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AN9">
         <v>0</v>
@@ -1532,13 +1443,13 @@
         <v>0</v>
       </c>
       <c r="AP9">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="AQ9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AR9">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="AS9">
         <v>0</v>
@@ -1549,73 +1460,85 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2005</v>
+        <v>2013</v>
       </c>
       <c r="B10">
-        <v>42.480762000166237</v>
+        <v>42.479828000262053</v>
       </c>
       <c r="C10">
-        <v>43.229126999711298</v>
+        <v>43.229155000103219</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10">
-        <v>3260</v>
+        <v>260</v>
       </c>
       <c r="F10">
-        <v>15890</v>
+        <v>74105</v>
       </c>
       <c r="G10">
-        <v>386530</v>
+        <v>300000</v>
+      </c>
+      <c r="H10">
+        <v>0.4</v>
+      </c>
+      <c r="I10">
+        <v>0.9</v>
+      </c>
+      <c r="J10">
+        <v>1.075</v>
       </c>
       <c r="K10">
-        <v>5920</v>
+        <v>24220</v>
       </c>
       <c r="L10">
-        <v>420</v>
+        <v>3210</v>
       </c>
       <c r="M10">
-        <v>0.47</v>
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="N10">
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="O10">
-        <v>0.16600000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="P10">
-        <v>5.37</v>
+        <v>11.6</v>
       </c>
       <c r="Q10">
-        <v>0.28000000000000003</v>
+        <v>0.67</v>
+      </c>
+      <c r="R10">
+        <v>0.17599999999999999</v>
       </c>
       <c r="S10">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="T10">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="U10">
-        <v>4.1799999999999997E-4</v>
+        <v>0.22</v>
       </c>
       <c r="V10">
-        <v>0.32</v>
+        <v>0.52</v>
       </c>
       <c r="W10">
-        <v>0.254</v>
-      </c>
-      <c r="X10">
-        <v>0.56999999999999995</v>
+        <v>0.91</v>
       </c>
       <c r="AA10">
-        <v>3.8000000000000002E-4</v>
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="AG10">
+        <v>2.63E-3</v>
       </c>
       <c r="AK10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AL10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN10">
         <v>0</v>
@@ -1624,10 +1547,10 @@
         <v>0</v>
       </c>
       <c r="AP10">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AQ10">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AR10">
         <v>16</v>
@@ -1641,79 +1564,82 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="B11">
-        <v>42.479376000102377</v>
+        <v>42.482537000182447</v>
       </c>
       <c r="C11">
-        <v>43.229760000123967</v>
+        <v>43.228182000199183</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="F11">
-        <v>138050</v>
+        <v>102150</v>
       </c>
       <c r="G11">
-        <v>228000</v>
+        <v>277779.99999999901</v>
       </c>
       <c r="K11">
-        <v>54330</v>
+        <v>184330</v>
       </c>
       <c r="L11">
-        <v>3450</v>
+        <v>4620</v>
       </c>
       <c r="M11">
-        <v>3.12</v>
+        <v>4.82</v>
+      </c>
+      <c r="N11">
+        <v>0.55000000000000004</v>
       </c>
       <c r="O11">
-        <v>6.14</v>
+        <v>1.84</v>
       </c>
       <c r="P11">
-        <v>423.4</v>
+        <v>51.52</v>
       </c>
       <c r="S11">
-        <v>1.375</v>
+        <v>0.33</v>
       </c>
       <c r="T11">
-        <v>2.91</v>
+        <v>1.03</v>
       </c>
       <c r="V11">
-        <v>0.82</v>
+        <v>0.67</v>
       </c>
       <c r="W11">
-        <v>1.835</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="AA11">
-        <v>3.28E-4</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AK11">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="AL11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP11">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="AQ11">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="AR11">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AS11">
         <v>0</v>
@@ -1724,85 +1650,76 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="B12">
-        <v>42.477304999925877</v>
+        <v>42.486509999936573</v>
       </c>
       <c r="C12">
-        <v>43.230735000120212</v>
+        <v>43.228030000384251</v>
       </c>
       <c r="D12" t="s">
         <v>50</v>
       </c>
       <c r="E12">
-        <v>4620</v>
+        <v>4104</v>
       </c>
       <c r="F12">
-        <v>65480.000000000007</v>
+        <v>60854</v>
       </c>
       <c r="G12">
-        <v>263339.99999999901</v>
+        <v>357220</v>
       </c>
       <c r="I12">
-        <v>1.07</v>
+        <v>0.23</v>
       </c>
       <c r="K12">
-        <v>14390</v>
+        <v>54930</v>
       </c>
       <c r="L12">
-        <v>9230</v>
+        <v>1330</v>
       </c>
       <c r="M12">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="N12">
-        <v>4.2999999999999997E-2</v>
+        <v>3.71</v>
       </c>
       <c r="O12">
-        <v>0.05</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="P12">
-        <v>3.5</v>
-      </c>
-      <c r="Q12">
-        <v>0.11</v>
-      </c>
-      <c r="R12">
-        <v>0.22</v>
+        <v>11.33</v>
       </c>
       <c r="S12">
-        <v>0.36</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="T12">
-        <v>0.25</v>
+        <v>0.44</v>
       </c>
       <c r="U12">
-        <v>5.1999999999999997E-5</v>
+        <v>3.5E-4</v>
       </c>
       <c r="V12">
-        <v>0.61</v>
+        <v>0.21</v>
       </c>
       <c r="W12">
-        <v>0.54</v>
+        <v>1.62</v>
       </c>
       <c r="X12">
-        <v>0.3</v>
-      </c>
-      <c r="AE12">
-        <v>2.21</v>
-      </c>
-      <c r="AF12">
-        <v>9.6299999999999999E-4</v>
+        <v>1.34</v>
+      </c>
+      <c r="Y12">
+        <v>1.48E-3</v>
+      </c>
+      <c r="Z12">
+        <v>1.91E-3</v>
       </c>
       <c r="AK12">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="AL12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AM12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AN12">
         <v>0</v>
@@ -1811,13 +1728,13 @@
         <v>0</v>
       </c>
       <c r="AP12">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="AQ12">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AR12">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AS12">
         <v>0</v>
@@ -1828,79 +1745,73 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2008</v>
+        <v>2017</v>
       </c>
       <c r="B13">
-        <v>42.476786000273762</v>
+        <v>42.480339000444587</v>
       </c>
       <c r="C13">
-        <v>43.231610000001517</v>
+        <v>43.229045000426481</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E13">
-        <v>14270</v>
+        <v>20540</v>
       </c>
       <c r="F13">
-        <v>104970</v>
+        <v>129500</v>
       </c>
       <c r="G13">
-        <v>270000</v>
+        <v>364900</v>
+      </c>
+      <c r="I13">
+        <v>0.47</v>
       </c>
       <c r="J13">
-        <v>1.1499999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="K13">
-        <v>53050</v>
+        <v>89900</v>
       </c>
       <c r="L13">
-        <v>7690</v>
+        <v>7720</v>
       </c>
       <c r="M13">
-        <v>6.14</v>
-      </c>
-      <c r="N13">
-        <v>0.67</v>
+        <v>12.44</v>
       </c>
       <c r="O13">
-        <v>2.12</v>
+        <v>1.71</v>
       </c>
       <c r="P13">
-        <v>84.26</v>
+        <v>110.15</v>
       </c>
       <c r="Q13">
-        <v>1.68</v>
-      </c>
-      <c r="R13">
-        <v>0.36</v>
+        <v>1.08</v>
       </c>
       <c r="S13">
-        <v>0.97</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T13">
-        <v>0.93</v>
-      </c>
-      <c r="U13">
-        <v>1.1E-4</v>
+        <v>0.45</v>
       </c>
       <c r="V13">
-        <v>0.62</v>
+        <v>1.05</v>
       </c>
       <c r="W13">
-        <v>4.1639999999999997</v>
-      </c>
-      <c r="X13">
-        <v>0.998</v>
+        <v>3.81</v>
+      </c>
+      <c r="AD13">
+        <v>1.624E-3</v>
       </c>
       <c r="AK13">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AL13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AM13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN13">
         <v>0</v>
@@ -1909,13 +1820,13 @@
         <v>0</v>
       </c>
       <c r="AP13">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AQ13">
         <v>10</v>
       </c>
       <c r="AR13">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="AS13">
         <v>0</v>
@@ -1926,85 +1837,106 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="B14">
-        <v>42.474755000143212</v>
+        <v>42.478301000000002</v>
       </c>
       <c r="C14">
-        <v>43.232109999676823</v>
+        <v>43.229779999999998</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E14">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="F14">
-        <v>181980</v>
+        <v>62680</v>
       </c>
       <c r="G14">
-        <v>246820</v>
+        <v>213700</v>
+      </c>
+      <c r="I14">
+        <v>0.5</v>
+      </c>
+      <c r="J14">
+        <v>0.96</v>
       </c>
       <c r="K14">
-        <v>121440</v>
+        <v>51310</v>
       </c>
       <c r="L14">
-        <v>890</v>
+        <v>4700</v>
       </c>
       <c r="M14">
-        <v>6.12</v>
+        <v>2.74</v>
       </c>
       <c r="N14">
-        <v>0.435</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O14">
-        <v>0.84</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="P14">
-        <v>67.7</v>
+        <v>41.65</v>
       </c>
       <c r="Q14">
-        <v>0.14000000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="R14">
-        <v>0.19800000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="S14">
-        <v>4.4999999999999998E-2</v>
+        <v>0.25</v>
       </c>
       <c r="T14">
-        <v>0.24199999999999999</v>
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="U14">
+        <v>2.63E-4</v>
       </c>
       <c r="V14">
-        <v>0.53300000000000003</v>
+        <v>0.62</v>
       </c>
       <c r="W14">
-        <v>3.8</v>
+        <v>1.67</v>
+      </c>
+      <c r="X14">
+        <v>1.04</v>
+      </c>
+      <c r="AA14">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB14">
+        <v>5.0500000000000002E-4</v>
+      </c>
+      <c r="AE14">
+        <v>0.86</v>
       </c>
       <c r="AK14">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="AL14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AM14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AO14">
         <v>0</v>
       </c>
       <c r="AP14">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="AQ14">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="AR14">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="AS14">
         <v>0</v>
@@ -2015,64 +1947,82 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2011</v>
+        <v>2018</v>
       </c>
       <c r="B15">
-        <v>42.477310000156422</v>
+        <v>42.479266000425639</v>
       </c>
       <c r="C15">
-        <v>43.229892999962033</v>
+        <v>43.229580999963218</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E15">
-        <v>370</v>
+        <v>1030</v>
       </c>
       <c r="F15">
-        <v>111090</v>
+        <v>46910</v>
       </c>
       <c r="G15">
-        <v>268620</v>
+        <v>209400</v>
       </c>
       <c r="K15">
-        <v>75540</v>
+        <v>20680</v>
       </c>
       <c r="L15">
-        <v>6970</v>
+        <v>1260</v>
       </c>
       <c r="M15">
-        <v>7.0990000000000002</v>
-      </c>
-      <c r="N15">
-        <v>0.62</v>
+        <v>1.05</v>
       </c>
       <c r="O15">
-        <v>1.37</v>
+        <v>0.85</v>
       </c>
       <c r="P15">
-        <v>92.25</v>
+        <v>12.41</v>
+      </c>
+      <c r="Q15">
+        <v>0.47</v>
       </c>
       <c r="S15">
-        <v>0.53</v>
+        <v>0.17</v>
       </c>
       <c r="T15">
-        <v>0.82</v>
+        <v>0.5</v>
+      </c>
+      <c r="U15">
+        <v>2.3E-5</v>
       </c>
       <c r="V15">
-        <v>0.76</v>
+        <v>1.34</v>
       </c>
       <c r="W15">
-        <v>3.25</v>
+        <v>0.18</v>
+      </c>
+      <c r="X15">
+        <v>1.25</v>
+      </c>
+      <c r="Y15">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="AA15">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="AC15">
+        <v>1.3700000000000001E-3</v>
+      </c>
+      <c r="AI15">
+        <v>1.9499999999999999E-3</v>
       </c>
       <c r="AK15">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="AL15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AM15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AN15">
         <v>0</v>
@@ -2081,13 +2031,13 @@
         <v>0</v>
       </c>
       <c r="AP15">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="AQ15">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AR15">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AS15">
         <v>0</v>
@@ -2098,86 +2048,77 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="B16">
-        <v>42.479828000262053</v>
+        <v>42.470527000320892</v>
       </c>
       <c r="C16">
-        <v>43.229155000103219</v>
+        <v>43.233797000131517</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E16">
-        <v>260</v>
+        <v>1260</v>
       </c>
       <c r="F16">
-        <v>74105</v>
+        <v>57630</v>
       </c>
       <c r="G16">
-        <v>300000</v>
-      </c>
-      <c r="H16">
-        <v>0.4</v>
-      </c>
-      <c r="I16">
-        <v>0.9</v>
-      </c>
-      <c r="J16">
-        <v>1.075</v>
+        <v>347830</v>
       </c>
       <c r="K16">
-        <v>24220</v>
+        <v>32700.000000000004</v>
       </c>
       <c r="L16">
-        <v>3210</v>
+        <v>645</v>
       </c>
       <c r="M16">
-        <v>0.57299999999999995</v>
-      </c>
-      <c r="N16">
-        <v>8.2000000000000003E-2</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="O16">
+        <v>0.71</v>
+      </c>
+      <c r="P16">
+        <v>7.38</v>
+      </c>
+      <c r="Q16">
+        <v>0.62</v>
+      </c>
+      <c r="R16">
+        <v>0.106</v>
+      </c>
+      <c r="S16">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="T16">
+        <v>1.87</v>
+      </c>
+      <c r="U16">
+        <v>2.7800000000000004E-4</v>
+      </c>
+      <c r="V16">
         <v>0.5</v>
       </c>
-      <c r="P16">
-        <v>11.6</v>
-      </c>
-      <c r="Q16">
-        <v>0.67</v>
-      </c>
-      <c r="R16">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="S16">
-        <v>0.25</v>
-      </c>
-      <c r="T16">
-        <v>0.22</v>
-      </c>
-      <c r="V16">
-        <v>0.52</v>
-      </c>
       <c r="W16">
-        <v>0.91</v>
-      </c>
-      <c r="AA16">
-        <v>5.4000000000000001E-4</v>
-      </c>
-      <c r="AG16">
-        <v>2.63E-3</v>
+        <v>0.311</v>
+      </c>
+      <c r="X16">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="AJ16">
+        <v>2.03E-4</v>
       </c>
       <c r="AK16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AL16">
+        <v>0</v>
+      </c>
+      <c r="AM16">
         <v>1</v>
       </c>
-      <c r="AM16">
-        <v>2</v>
-      </c>
       <c r="AN16">
         <v>0</v>
       </c>
@@ -2185,13 +2126,13 @@
         <v>0</v>
       </c>
       <c r="AP16">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AQ16">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="AR16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -2200,468 +2141,77 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2014</v>
-      </c>
-      <c r="B17">
-        <v>42.482537000182447</v>
-      </c>
-      <c r="C17">
-        <v>43.228182000199183</v>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>3000</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17">
-        <v>230</v>
-      </c>
-      <c r="F17">
-        <v>102150</v>
-      </c>
-      <c r="G17">
-        <v>277779.99999999901</v>
-      </c>
-      <c r="K17">
-        <v>184330</v>
-      </c>
-      <c r="L17">
-        <v>4620</v>
-      </c>
-      <c r="M17">
-        <v>4.82</v>
-      </c>
-      <c r="N17">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="O17">
-        <v>1.84</v>
-      </c>
-      <c r="P17">
-        <v>51.52</v>
-      </c>
-      <c r="S17">
-        <v>0.33</v>
-      </c>
-      <c r="T17">
-        <v>1.03</v>
-      </c>
-      <c r="V17">
-        <v>0.67</v>
-      </c>
-      <c r="W17">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="AA17">
-        <v>1.07E-3</v>
-      </c>
-      <c r="AK17">
-        <v>29</v>
-      </c>
-      <c r="AL17">
-        <v>4</v>
-      </c>
-      <c r="AM17">
-        <v>4</v>
-      </c>
-      <c r="AN17">
-        <v>3</v>
-      </c>
-      <c r="AO17">
-        <v>0</v>
-      </c>
-      <c r="AP17">
-        <v>34</v>
-      </c>
-      <c r="AQ17">
-        <v>6</v>
-      </c>
-      <c r="AR17">
-        <v>20</v>
-      </c>
-      <c r="AS17">
-        <v>0</v>
-      </c>
-      <c r="AT17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2017</v>
-      </c>
-      <c r="B18">
-        <v>42.480339000444587</v>
-      </c>
-      <c r="C18">
-        <v>43.229045000426481</v>
-      </c>
-      <c r="D18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18">
-        <v>20540</v>
-      </c>
-      <c r="F18">
-        <v>129500</v>
-      </c>
-      <c r="G18">
-        <v>364900</v>
-      </c>
-      <c r="I18">
-        <v>0.47</v>
-      </c>
-      <c r="J18">
-        <v>0.96</v>
-      </c>
-      <c r="K18">
-        <v>89900</v>
-      </c>
-      <c r="L18">
-        <v>7720</v>
-      </c>
-      <c r="M18">
-        <v>12.44</v>
-      </c>
-      <c r="O18">
-        <v>1.71</v>
-      </c>
-      <c r="P18">
-        <v>110.15</v>
-      </c>
-      <c r="Q18">
-        <v>1.08</v>
-      </c>
-      <c r="S18">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="T18">
-        <v>0.45</v>
-      </c>
-      <c r="V18">
-        <v>1.05</v>
-      </c>
-      <c r="W18">
-        <v>3.81</v>
-      </c>
-      <c r="AD18">
-        <v>1.624E-3</v>
-      </c>
-      <c r="AK18">
-        <v>15</v>
-      </c>
-      <c r="AL18">
-        <v>2</v>
-      </c>
-      <c r="AM18">
-        <v>3</v>
-      </c>
-      <c r="AN18">
-        <v>0</v>
-      </c>
-      <c r="AO18">
-        <v>0</v>
-      </c>
-      <c r="AP18">
-        <v>52</v>
-      </c>
-      <c r="AQ18">
-        <v>10</v>
-      </c>
-      <c r="AR18">
-        <v>18</v>
-      </c>
-      <c r="AS18">
-        <v>0</v>
-      </c>
-      <c r="AT18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2015</v>
-      </c>
-      <c r="B19">
-        <v>42.485105309262678</v>
-      </c>
-      <c r="C19">
-        <v>43.227299262550957</v>
-      </c>
-      <c r="D19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19">
-        <v>50</v>
-      </c>
-      <c r="F19">
-        <v>11280</v>
-      </c>
-      <c r="G19">
-        <v>155000</v>
-      </c>
-      <c r="K19">
-        <v>5650</v>
-      </c>
-      <c r="L19">
-        <v>580</v>
-      </c>
-      <c r="M19">
-        <v>0.34</v>
-      </c>
-      <c r="O19">
-        <v>0.122</v>
-      </c>
-      <c r="P19">
-        <v>4.75</v>
-      </c>
-      <c r="Q19">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="R19">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="S19">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="T19">
-        <v>0.17399999999999899</v>
-      </c>
-      <c r="V19">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="W19">
-        <v>0.17</v>
-      </c>
-      <c r="AD19">
-        <v>6.8000000000000005E-4</v>
-      </c>
-      <c r="AK19">
-        <v>4</v>
-      </c>
-      <c r="AL19">
-        <v>0</v>
-      </c>
-      <c r="AM19">
-        <v>1</v>
-      </c>
-      <c r="AN19">
-        <v>0</v>
-      </c>
-      <c r="AO19">
-        <v>0</v>
-      </c>
-      <c r="AP19">
-        <v>70</v>
-      </c>
-      <c r="AQ19">
-        <v>9</v>
-      </c>
-      <c r="AR19">
-        <v>16</v>
-      </c>
-      <c r="AS19">
-        <v>0</v>
-      </c>
-      <c r="AT19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>2001</v>
-      </c>
-      <c r="B20">
-        <v>42.486509999936573</v>
-      </c>
-      <c r="C20">
-        <v>43.228030000384251</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20">
-        <v>4104</v>
-      </c>
-      <c r="F20">
-        <v>60854</v>
-      </c>
-      <c r="G20">
-        <v>357220</v>
-      </c>
-      <c r="I20">
-        <v>0.23</v>
-      </c>
-      <c r="K20">
-        <v>54930</v>
-      </c>
-      <c r="L20">
-        <v>1330</v>
-      </c>
-      <c r="M20">
-        <v>3.71</v>
-      </c>
-      <c r="O20">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="P20">
-        <v>11.33</v>
-      </c>
-      <c r="S20">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="T20">
-        <v>0.44</v>
-      </c>
-      <c r="U20">
-        <v>3.5E-4</v>
-      </c>
-      <c r="V20">
-        <v>0.21</v>
-      </c>
-      <c r="W20">
-        <v>1.62</v>
-      </c>
-      <c r="X20">
-        <v>1.34</v>
-      </c>
-      <c r="Y20">
-        <v>1.48E-3</v>
-      </c>
-      <c r="Z20">
-        <v>1.91E-3</v>
-      </c>
-      <c r="AK20">
-        <v>32</v>
-      </c>
-      <c r="AL20">
-        <v>7</v>
-      </c>
-      <c r="AM20">
-        <v>4</v>
-      </c>
-      <c r="AN20">
-        <v>0</v>
-      </c>
-      <c r="AO20">
-        <v>0</v>
-      </c>
-      <c r="AP20">
-        <v>42</v>
-      </c>
-      <c r="AQ20">
-        <v>0</v>
-      </c>
-      <c r="AR20">
-        <v>15</v>
-      </c>
-      <c r="AS20">
-        <v>0</v>
-      </c>
-      <c r="AT20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>3000</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3">
+        <v>51</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
         <f>5.03*1000</f>
         <v>5030</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G17" s="3">
         <f>427.3*1000</f>
         <v>427300</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H17" s="3">
         <v>0.9</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3">
         <f>3.68*1000</f>
         <v>3680</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L17" s="3">
         <f>2.9*1000</f>
         <v>2900</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M17" s="3">
         <v>0.81</v>
       </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3">
+      <c r="N17" s="3"/>
+      <c r="O17" s="3">
         <f>2.1/1000</f>
         <v>2.1000000000000003E-3</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P17" s="3">
         <v>12.35</v>
       </c>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3">
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3">
         <v>1.2</v>
       </c>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3">
+      <c r="U17" s="3"/>
+      <c r="V17" s="3">
         <v>0.3</v>
       </c>
-      <c r="W21" s="3">
+      <c r="W17" s="3">
         <v>0.6</v>
       </c>
-      <c r="AK21" s="3">
+      <c r="AK17" s="3">
         <v>9</v>
       </c>
-      <c r="AL21" s="3"/>
-      <c r="AM21" s="3">
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3">
         <v>2</v>
       </c>
-      <c r="AP21" s="3">
+      <c r="AP17" s="3">
         <v>59</v>
       </c>
-      <c r="AQ21" s="3">
+      <c r="AQ17" s="3">
         <v>13</v>
       </c>
-      <c r="AR21" s="3">
+      <c r="AR17" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="AK22" s="3"/>
-      <c r="AL22" s="3"/>
-      <c r="AM22" s="3"/>
-      <c r="AP22" s="3"/>
-      <c r="AQ22" s="3"/>
-      <c r="AR22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
results are not so good
</commit_message>
<xml_diff>
--- a/North_Valley/data/North_Valley_Data.xlsx
+++ b/North_Valley/data/North_Valley_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT17"/>
+  <dimension ref="A1:AT23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,79 +1190,73 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="B7">
-        <v>42.476786000273762</v>
+        <v>42.480762000166237</v>
       </c>
       <c r="C7">
-        <v>43.231610000001517</v>
+        <v>43.229126999711298</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
       </c>
       <c r="E7">
-        <v>14270</v>
+        <v>3260</v>
       </c>
       <c r="F7">
-        <v>104970</v>
+        <v>15890</v>
       </c>
       <c r="G7">
-        <v>270000</v>
-      </c>
-      <c r="J7">
-        <v>1.1499999999999999</v>
+        <v>386530</v>
       </c>
       <c r="K7">
-        <v>53050</v>
+        <v>5920</v>
       </c>
       <c r="L7">
-        <v>7690</v>
+        <v>420</v>
       </c>
       <c r="M7">
-        <v>6.14</v>
-      </c>
-      <c r="N7">
-        <v>0.67</v>
+        <v>0.47</v>
       </c>
       <c r="O7">
-        <v>2.12</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="P7">
-        <v>84.26</v>
+        <v>5.37</v>
       </c>
       <c r="Q7">
-        <v>1.68</v>
-      </c>
-      <c r="R7">
-        <v>0.36</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="S7">
-        <v>0.97</v>
+        <v>0.1</v>
       </c>
       <c r="T7">
-        <v>0.93</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="U7">
-        <v>1.1E-4</v>
+        <v>4.1799999999999997E-4</v>
       </c>
       <c r="V7">
-        <v>0.62</v>
+        <v>0.32</v>
       </c>
       <c r="W7">
-        <v>4.1639999999999997</v>
+        <v>0.254</v>
       </c>
       <c r="X7">
-        <v>0.998</v>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AA7">
+        <v>3.8000000000000002E-4</v>
       </c>
       <c r="AK7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AL7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AM7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN7">
         <v>0</v>
@@ -1271,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="AP7">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AQ7">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AR7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AS7">
         <v>0</v>
@@ -1288,85 +1282,79 @@
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B8">
-        <v>42.474755000143212</v>
+        <v>42.479376000102377</v>
       </c>
       <c r="C8">
-        <v>43.232109999676823</v>
+        <v>43.229760000123967</v>
       </c>
       <c r="D8" t="s">
         <v>50</v>
       </c>
       <c r="E8">
-        <v>83</v>
+        <v>240</v>
       </c>
       <c r="F8">
-        <v>181980</v>
+        <v>138050</v>
       </c>
       <c r="G8">
-        <v>246820</v>
+        <v>228000</v>
       </c>
       <c r="K8">
-        <v>121440</v>
+        <v>54330</v>
       </c>
       <c r="L8">
-        <v>890</v>
+        <v>3450</v>
       </c>
       <c r="M8">
-        <v>6.12</v>
-      </c>
-      <c r="N8">
-        <v>0.435</v>
+        <v>3.12</v>
       </c>
       <c r="O8">
-        <v>0.84</v>
+        <v>6.14</v>
       </c>
       <c r="P8">
-        <v>67.7</v>
-      </c>
-      <c r="Q8">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R8">
-        <v>0.19800000000000001</v>
+        <v>423.4</v>
       </c>
       <c r="S8">
-        <v>4.4999999999999998E-2</v>
+        <v>1.375</v>
       </c>
       <c r="T8">
-        <v>0.24199999999999999</v>
+        <v>2.91</v>
       </c>
       <c r="V8">
-        <v>0.53300000000000003</v>
+        <v>0.82</v>
       </c>
       <c r="W8">
-        <v>3.8</v>
+        <v>1.835</v>
+      </c>
+      <c r="AA8">
+        <v>3.28E-4</v>
       </c>
       <c r="AK8">
+        <v>18</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>2</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8">
         <v>51</v>
       </c>
-      <c r="AL8">
-        <v>1</v>
-      </c>
-      <c r="AM8">
-        <v>3</v>
-      </c>
-      <c r="AN8">
-        <v>7</v>
-      </c>
-      <c r="AO8">
-        <v>0</v>
-      </c>
-      <c r="AP8">
-        <v>30</v>
-      </c>
       <c r="AQ8">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="AR8">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="AS8">
         <v>0</v>
@@ -1377,64 +1365,85 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="B9">
-        <v>42.477310000156422</v>
+        <v>42.477304999925877</v>
       </c>
       <c r="C9">
-        <v>43.229892999962033</v>
+        <v>43.230735000120212</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9">
-        <v>370</v>
+        <v>4620</v>
       </c>
       <c r="F9">
-        <v>111090</v>
+        <v>65480.000000000007</v>
       </c>
       <c r="G9">
-        <v>268620</v>
+        <v>263339.99999999901</v>
+      </c>
+      <c r="I9">
+        <v>1.07</v>
       </c>
       <c r="K9">
-        <v>75540</v>
+        <v>14390</v>
       </c>
       <c r="L9">
-        <v>6970</v>
+        <v>9230</v>
       </c>
       <c r="M9">
-        <v>7.0990000000000002</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="N9">
-        <v>0.62</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="O9">
-        <v>1.37</v>
+        <v>0.05</v>
       </c>
       <c r="P9">
-        <v>92.25</v>
+        <v>3.5</v>
+      </c>
+      <c r="Q9">
+        <v>0.11</v>
+      </c>
+      <c r="R9">
+        <v>0.22</v>
       </c>
       <c r="S9">
-        <v>0.53</v>
+        <v>0.36</v>
       </c>
       <c r="T9">
-        <v>0.82</v>
+        <v>0.25</v>
+      </c>
+      <c r="U9">
+        <v>5.1999999999999997E-5</v>
       </c>
       <c r="V9">
-        <v>0.76</v>
+        <v>0.61</v>
       </c>
       <c r="W9">
-        <v>3.25</v>
+        <v>0.54</v>
+      </c>
+      <c r="X9">
+        <v>0.3</v>
+      </c>
+      <c r="AE9">
+        <v>2.21</v>
+      </c>
+      <c r="AF9">
+        <v>9.6299999999999999E-4</v>
       </c>
       <c r="AK9">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AL9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AM9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AN9">
         <v>0</v>
@@ -1443,13 +1452,13 @@
         <v>0</v>
       </c>
       <c r="AP9">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="AQ9">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AR9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AS9">
         <v>0</v>
@@ -1460,85 +1469,79 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="B10">
-        <v>42.479828000262053</v>
+        <v>42.476786000273762</v>
       </c>
       <c r="C10">
-        <v>43.229155000103219</v>
+        <v>43.231610000001517</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E10">
-        <v>260</v>
+        <v>14270</v>
       </c>
       <c r="F10">
-        <v>74105</v>
+        <v>104970</v>
       </c>
       <c r="G10">
-        <v>300000</v>
-      </c>
-      <c r="H10">
-        <v>0.4</v>
-      </c>
-      <c r="I10">
-        <v>0.9</v>
+        <v>270000</v>
       </c>
       <c r="J10">
-        <v>1.075</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K10">
-        <v>24220</v>
+        <v>53050</v>
       </c>
       <c r="L10">
-        <v>3210</v>
+        <v>7690</v>
       </c>
       <c r="M10">
-        <v>0.57299999999999995</v>
+        <v>6.14</v>
       </c>
       <c r="N10">
-        <v>8.2000000000000003E-2</v>
+        <v>0.67</v>
       </c>
       <c r="O10">
-        <v>0.5</v>
+        <v>2.12</v>
       </c>
       <c r="P10">
-        <v>11.6</v>
+        <v>84.26</v>
       </c>
       <c r="Q10">
-        <v>0.67</v>
+        <v>1.68</v>
       </c>
       <c r="R10">
-        <v>0.17599999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="S10">
-        <v>0.25</v>
+        <v>0.97</v>
       </c>
       <c r="T10">
-        <v>0.22</v>
+        <v>0.93</v>
+      </c>
+      <c r="U10">
+        <v>1.1E-4</v>
       </c>
       <c r="V10">
-        <v>0.52</v>
+        <v>0.62</v>
       </c>
       <c r="W10">
-        <v>0.91</v>
-      </c>
-      <c r="AA10">
-        <v>5.4000000000000001E-4</v>
-      </c>
-      <c r="AG10">
-        <v>2.63E-3</v>
+        <v>4.1639999999999997</v>
+      </c>
+      <c r="X10">
+        <v>0.998</v>
       </c>
       <c r="AK10">
         <v>10</v>
       </c>
       <c r="AL10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AM10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN10">
         <v>0</v>
@@ -1547,13 +1550,13 @@
         <v>0</v>
       </c>
       <c r="AP10">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AQ10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AR10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AS10">
         <v>0</v>
@@ -1564,82 +1567,85 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="B11">
-        <v>42.482537000182447</v>
+        <v>42.474755000143212</v>
       </c>
       <c r="C11">
-        <v>43.228182000199183</v>
+        <v>43.232109999676823</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11">
-        <v>230</v>
+        <v>83</v>
       </c>
       <c r="F11">
-        <v>102150</v>
+        <v>181980</v>
       </c>
       <c r="G11">
-        <v>277779.99999999901</v>
+        <v>246820</v>
       </c>
       <c r="K11">
-        <v>184330</v>
+        <v>121440</v>
       </c>
       <c r="L11">
-        <v>4620</v>
+        <v>890</v>
       </c>
       <c r="M11">
-        <v>4.82</v>
+        <v>6.12</v>
       </c>
       <c r="N11">
-        <v>0.55000000000000004</v>
+        <v>0.435</v>
       </c>
       <c r="O11">
-        <v>1.84</v>
+        <v>0.84</v>
       </c>
       <c r="P11">
-        <v>51.52</v>
+        <v>67.7</v>
+      </c>
+      <c r="Q11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R11">
+        <v>0.19800000000000001</v>
       </c>
       <c r="S11">
-        <v>0.33</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="T11">
-        <v>1.03</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="V11">
-        <v>0.67</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="W11">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="AA11">
-        <v>1.07E-3</v>
+        <v>3.8</v>
       </c>
       <c r="AK11">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="AL11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AM11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AO11">
         <v>0</v>
       </c>
       <c r="AP11">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AQ11">
+        <v>2</v>
+      </c>
+      <c r="AR11">
         <v>6</v>
-      </c>
-      <c r="AR11">
-        <v>20</v>
       </c>
       <c r="AS11">
         <v>0</v>
@@ -1650,76 +1656,64 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2001</v>
+        <v>2011</v>
       </c>
       <c r="B12">
-        <v>42.486509999936573</v>
+        <v>42.477310000156422</v>
       </c>
       <c r="C12">
-        <v>43.228030000384251</v>
+        <v>43.229892999962033</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12">
-        <v>4104</v>
+        <v>370</v>
       </c>
       <c r="F12">
-        <v>60854</v>
+        <v>111090</v>
       </c>
       <c r="G12">
-        <v>357220</v>
-      </c>
-      <c r="I12">
-        <v>0.23</v>
+        <v>268620</v>
       </c>
       <c r="K12">
-        <v>54930</v>
+        <v>75540</v>
       </c>
       <c r="L12">
-        <v>1330</v>
+        <v>6970</v>
       </c>
       <c r="M12">
-        <v>3.71</v>
+        <v>7.0990000000000002</v>
+      </c>
+      <c r="N12">
+        <v>0.62</v>
       </c>
       <c r="O12">
-        <v>0.82299999999999995</v>
+        <v>1.37</v>
       </c>
       <c r="P12">
-        <v>11.33</v>
+        <v>92.25</v>
       </c>
       <c r="S12">
-        <v>0.25700000000000001</v>
+        <v>0.53</v>
       </c>
       <c r="T12">
-        <v>0.44</v>
-      </c>
-      <c r="U12">
-        <v>3.5E-4</v>
+        <v>0.82</v>
       </c>
       <c r="V12">
-        <v>0.21</v>
+        <v>0.76</v>
       </c>
       <c r="W12">
-        <v>1.62</v>
-      </c>
-      <c r="X12">
-        <v>1.34</v>
-      </c>
-      <c r="Y12">
-        <v>1.48E-3</v>
-      </c>
-      <c r="Z12">
-        <v>1.91E-3</v>
+        <v>3.25</v>
       </c>
       <c r="AK12">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="AL12">
         <v>7</v>
       </c>
       <c r="AM12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AN12">
         <v>0</v>
@@ -1728,13 +1722,13 @@
         <v>0</v>
       </c>
       <c r="AP12">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="AQ12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AR12">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AS12">
         <v>0</v>
@@ -1745,74 +1739,86 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="B13">
-        <v>42.480339000444587</v>
+        <v>42.479828000262053</v>
       </c>
       <c r="C13">
-        <v>43.229045000426481</v>
+        <v>43.229155000103219</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13">
-        <v>20540</v>
+        <v>260</v>
       </c>
       <c r="F13">
-        <v>129500</v>
+        <v>74105</v>
       </c>
       <c r="G13">
-        <v>364900</v>
+        <v>300000</v>
+      </c>
+      <c r="H13">
+        <v>0.4</v>
       </c>
       <c r="I13">
-        <v>0.47</v>
+        <v>0.9</v>
       </c>
       <c r="J13">
-        <v>0.96</v>
+        <v>1.075</v>
       </c>
       <c r="K13">
-        <v>89900</v>
+        <v>24220</v>
       </c>
       <c r="L13">
-        <v>7720</v>
+        <v>3210</v>
       </c>
       <c r="M13">
-        <v>12.44</v>
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="N13">
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="O13">
-        <v>1.71</v>
+        <v>0.5</v>
       </c>
       <c r="P13">
-        <v>110.15</v>
+        <v>11.6</v>
       </c>
       <c r="Q13">
-        <v>1.08</v>
+        <v>0.67</v>
+      </c>
+      <c r="R13">
+        <v>0.17599999999999999</v>
       </c>
       <c r="S13">
-        <v>0.55000000000000004</v>
+        <v>0.25</v>
       </c>
       <c r="T13">
-        <v>0.45</v>
+        <v>0.22</v>
       </c>
       <c r="V13">
-        <v>1.05</v>
+        <v>0.52</v>
       </c>
       <c r="W13">
-        <v>3.81</v>
-      </c>
-      <c r="AD13">
-        <v>1.624E-3</v>
+        <v>0.91</v>
+      </c>
+      <c r="AA13">
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="AG13">
+        <v>2.63E-3</v>
       </c>
       <c r="AK13">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AL13">
+        <v>1</v>
+      </c>
+      <c r="AM13">
         <v>2</v>
       </c>
-      <c r="AM13">
-        <v>3</v>
-      </c>
       <c r="AN13">
         <v>0</v>
       </c>
@@ -1820,13 +1826,13 @@
         <v>0</v>
       </c>
       <c r="AP13">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="AQ13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AR13">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AS13">
         <v>0</v>
@@ -1837,106 +1843,82 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="B14">
-        <v>42.478301000000002</v>
+        <v>42.482537000182447</v>
       </c>
       <c r="C14">
-        <v>43.229779999999998</v>
+        <v>43.228182000199183</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14">
-        <v>125</v>
+        <v>230</v>
       </c>
       <c r="F14">
-        <v>62680</v>
+        <v>102150</v>
       </c>
       <c r="G14">
-        <v>213700</v>
-      </c>
-      <c r="I14">
-        <v>0.5</v>
-      </c>
-      <c r="J14">
-        <v>0.96</v>
+        <v>277779.99999999901</v>
       </c>
       <c r="K14">
-        <v>51310</v>
+        <v>184330</v>
       </c>
       <c r="L14">
-        <v>4700</v>
+        <v>4620</v>
       </c>
       <c r="M14">
-        <v>2.74</v>
+        <v>4.82</v>
       </c>
       <c r="N14">
-        <v>7.4999999999999997E-2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O14">
-        <v>0.63500000000000001</v>
+        <v>1.84</v>
       </c>
       <c r="P14">
-        <v>41.65</v>
-      </c>
-      <c r="Q14">
-        <v>0.73</v>
-      </c>
-      <c r="R14">
-        <v>0.13500000000000001</v>
+        <v>51.52</v>
       </c>
       <c r="S14">
-        <v>0.25</v>
+        <v>0.33</v>
       </c>
       <c r="T14">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="U14">
-        <v>2.63E-4</v>
+        <v>1.03</v>
       </c>
       <c r="V14">
-        <v>0.62</v>
+        <v>0.67</v>
       </c>
       <c r="W14">
-        <v>1.67</v>
-      </c>
-      <c r="X14">
-        <v>1.04</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="AA14">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="AB14">
-        <v>5.0500000000000002E-4</v>
-      </c>
-      <c r="AE14">
-        <v>0.86</v>
+        <v>1.07E-3</v>
       </c>
       <c r="AK14">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="AL14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO14">
         <v>0</v>
       </c>
       <c r="AP14">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="AQ14">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="AR14">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="AS14">
         <v>0</v>
@@ -1947,82 +1929,76 @@
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2018</v>
+        <v>2001</v>
       </c>
       <c r="B15">
-        <v>42.479266000425639</v>
+        <v>42.486509999936573</v>
       </c>
       <c r="C15">
-        <v>43.229580999963218</v>
+        <v>43.228030000384251</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15">
-        <v>1030</v>
+        <v>4104</v>
       </c>
       <c r="F15">
-        <v>46910</v>
+        <v>60854</v>
       </c>
       <c r="G15">
-        <v>209400</v>
+        <v>357220</v>
+      </c>
+      <c r="I15">
+        <v>0.23</v>
       </c>
       <c r="K15">
-        <v>20680</v>
+        <v>54930</v>
       </c>
       <c r="L15">
-        <v>1260</v>
+        <v>1330</v>
       </c>
       <c r="M15">
-        <v>1.05</v>
+        <v>3.71</v>
       </c>
       <c r="O15">
-        <v>0.85</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="P15">
-        <v>12.41</v>
-      </c>
-      <c r="Q15">
-        <v>0.47</v>
+        <v>11.33</v>
       </c>
       <c r="S15">
-        <v>0.17</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="T15">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
       <c r="U15">
-        <v>2.3E-5</v>
+        <v>3.5E-4</v>
       </c>
       <c r="V15">
+        <v>0.21</v>
+      </c>
+      <c r="W15">
+        <v>1.62</v>
+      </c>
+      <c r="X15">
         <v>1.34</v>
       </c>
-      <c r="W15">
-        <v>0.18</v>
-      </c>
-      <c r="X15">
-        <v>1.25</v>
-      </c>
       <c r="Y15">
-        <v>1.5200000000000001E-3</v>
-      </c>
-      <c r="AA15">
-        <v>4.4000000000000002E-4</v>
-      </c>
-      <c r="AC15">
-        <v>1.3700000000000001E-3</v>
-      </c>
-      <c r="AI15">
-        <v>1.9499999999999999E-3</v>
+        <v>1.48E-3</v>
+      </c>
+      <c r="Z15">
+        <v>1.91E-3</v>
       </c>
       <c r="AK15">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="AL15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AM15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN15">
         <v>0</v>
@@ -2031,13 +2007,13 @@
         <v>0</v>
       </c>
       <c r="AP15">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="AQ15">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AR15">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AS15">
         <v>0</v>
@@ -2048,168 +2024,633 @@
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="B16">
-        <v>42.470527000320892</v>
+        <v>42.480339000444587</v>
       </c>
       <c r="C16">
-        <v>43.233797000131517</v>
+        <v>43.229045000426481</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
       </c>
       <c r="E16">
+        <v>20540</v>
+      </c>
+      <c r="F16">
+        <v>129500</v>
+      </c>
+      <c r="G16">
+        <v>364900</v>
+      </c>
+      <c r="I16">
+        <v>0.47</v>
+      </c>
+      <c r="J16">
+        <v>0.96</v>
+      </c>
+      <c r="K16">
+        <v>89900</v>
+      </c>
+      <c r="L16">
+        <v>7720</v>
+      </c>
+      <c r="M16">
+        <v>12.44</v>
+      </c>
+      <c r="O16">
+        <v>1.71</v>
+      </c>
+      <c r="P16">
+        <v>110.15</v>
+      </c>
+      <c r="Q16">
+        <v>1.08</v>
+      </c>
+      <c r="S16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T16">
+        <v>0.45</v>
+      </c>
+      <c r="V16">
+        <v>1.05</v>
+      </c>
+      <c r="W16">
+        <v>3.81</v>
+      </c>
+      <c r="AD16">
+        <v>1.624E-3</v>
+      </c>
+      <c r="AK16">
+        <v>15</v>
+      </c>
+      <c r="AL16">
+        <v>2</v>
+      </c>
+      <c r="AM16">
+        <v>3</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>52</v>
+      </c>
+      <c r="AQ16">
+        <v>10</v>
+      </c>
+      <c r="AR16">
+        <v>18</v>
+      </c>
+      <c r="AS16">
+        <v>0</v>
+      </c>
+      <c r="AT16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2012</v>
+      </c>
+      <c r="B17">
+        <v>42.478301000000002</v>
+      </c>
+      <c r="C17">
+        <v>43.229779999999998</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>125</v>
+      </c>
+      <c r="F17">
+        <v>62680</v>
+      </c>
+      <c r="G17">
+        <v>213700</v>
+      </c>
+      <c r="I17">
+        <v>0.5</v>
+      </c>
+      <c r="J17">
+        <v>0.96</v>
+      </c>
+      <c r="K17">
+        <v>51310</v>
+      </c>
+      <c r="L17">
+        <v>4700</v>
+      </c>
+      <c r="M17">
+        <v>2.74</v>
+      </c>
+      <c r="N17">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="O17">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="P17">
+        <v>41.65</v>
+      </c>
+      <c r="Q17">
+        <v>0.73</v>
+      </c>
+      <c r="R17">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="S17">
+        <v>0.25</v>
+      </c>
+      <c r="T17">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="U17">
+        <v>2.63E-4</v>
+      </c>
+      <c r="V17">
+        <v>0.62</v>
+      </c>
+      <c r="W17">
+        <v>1.67</v>
+      </c>
+      <c r="X17">
+        <v>1.04</v>
+      </c>
+      <c r="AA17">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB17">
+        <v>5.0500000000000002E-4</v>
+      </c>
+      <c r="AE17">
+        <v>0.86</v>
+      </c>
+      <c r="AK17">
+        <v>16</v>
+      </c>
+      <c r="AL17">
+        <v>5</v>
+      </c>
+      <c r="AM17">
+        <v>2</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>53</v>
+      </c>
+      <c r="AQ17">
+        <v>11</v>
+      </c>
+      <c r="AR17">
+        <v>13</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2018</v>
+      </c>
+      <c r="B18">
+        <v>42.479266000425639</v>
+      </c>
+      <c r="C18">
+        <v>43.229580999963218</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18">
+        <v>1030</v>
+      </c>
+      <c r="F18">
+        <v>46910</v>
+      </c>
+      <c r="G18">
+        <v>209400</v>
+      </c>
+      <c r="K18">
+        <v>20680</v>
+      </c>
+      <c r="L18">
         <v>1260</v>
       </c>
-      <c r="F16">
+      <c r="M18">
+        <v>1.05</v>
+      </c>
+      <c r="O18">
+        <v>0.85</v>
+      </c>
+      <c r="P18">
+        <v>12.41</v>
+      </c>
+      <c r="Q18">
+        <v>0.47</v>
+      </c>
+      <c r="S18">
+        <v>0.17</v>
+      </c>
+      <c r="T18">
+        <v>0.5</v>
+      </c>
+      <c r="U18">
+        <v>2.3E-5</v>
+      </c>
+      <c r="V18">
+        <v>1.34</v>
+      </c>
+      <c r="W18">
+        <v>0.18</v>
+      </c>
+      <c r="X18">
+        <v>1.25</v>
+      </c>
+      <c r="Y18">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="AA18">
+        <v>4.4000000000000002E-4</v>
+      </c>
+      <c r="AC18">
+        <v>1.3700000000000001E-3</v>
+      </c>
+      <c r="AI18">
+        <v>1.9499999999999999E-3</v>
+      </c>
+      <c r="AK18">
+        <v>11</v>
+      </c>
+      <c r="AL18">
+        <v>2</v>
+      </c>
+      <c r="AM18">
+        <v>2</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>57</v>
+      </c>
+      <c r="AQ18">
+        <v>11</v>
+      </c>
+      <c r="AR18">
+        <v>17</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2010</v>
+      </c>
+      <c r="B19">
+        <v>42.470527000320892</v>
+      </c>
+      <c r="C19">
+        <v>43.233797000131517</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19">
+        <v>1260</v>
+      </c>
+      <c r="F19">
         <v>57630</v>
       </c>
-      <c r="G16">
+      <c r="G19">
         <v>347830</v>
       </c>
-      <c r="K16">
+      <c r="K19">
         <v>32700.000000000004</v>
       </c>
-      <c r="L16">
+      <c r="L19">
         <v>645</v>
       </c>
-      <c r="M16">
+      <c r="M19">
         <v>0.68899999999999995</v>
       </c>
-      <c r="O16">
+      <c r="O19">
         <v>0.71</v>
       </c>
-      <c r="P16">
+      <c r="P19">
         <v>7.38</v>
       </c>
-      <c r="Q16">
+      <c r="Q19">
         <v>0.62</v>
       </c>
-      <c r="R16">
+      <c r="R19">
         <v>0.106</v>
       </c>
-      <c r="S16">
+      <c r="S19">
         <v>0.14499999999999999</v>
       </c>
-      <c r="T16">
+      <c r="T19">
         <v>1.87</v>
       </c>
-      <c r="U16">
+      <c r="U19">
         <v>2.7800000000000004E-4</v>
       </c>
-      <c r="V16">
+      <c r="V19">
         <v>0.5</v>
       </c>
-      <c r="W16">
+      <c r="W19">
         <v>0.311</v>
       </c>
-      <c r="X16">
+      <c r="X19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="AJ16">
+      <c r="AJ19">
         <v>2.03E-4</v>
       </c>
-      <c r="AK16">
+      <c r="AK19">
         <v>9</v>
       </c>
-      <c r="AL16">
-        <v>0</v>
-      </c>
-      <c r="AM16">
+      <c r="AL19">
+        <v>0</v>
+      </c>
+      <c r="AM19">
         <v>1</v>
       </c>
-      <c r="AN16">
-        <v>0</v>
-      </c>
-      <c r="AO16">
-        <v>0</v>
-      </c>
-      <c r="AP16">
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
+        <v>0</v>
+      </c>
+      <c r="AP19">
         <v>57</v>
       </c>
-      <c r="AQ16">
+      <c r="AQ19">
         <v>16</v>
       </c>
-      <c r="AR16">
+      <c r="AR19">
         <v>17</v>
       </c>
-      <c r="AS16">
-        <v>0</v>
-      </c>
-      <c r="AT16">
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2015</v>
+      </c>
+      <c r="B20">
+        <v>42.485105309262678</v>
+      </c>
+      <c r="C20">
+        <v>43.227299262550957</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20">
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>11280</v>
+      </c>
+      <c r="G20">
+        <v>155000</v>
+      </c>
+      <c r="K20">
+        <v>5650</v>
+      </c>
+      <c r="L20">
+        <v>580</v>
+      </c>
+      <c r="M20">
+        <v>0.34</v>
+      </c>
+      <c r="O20">
+        <v>0.122</v>
+      </c>
+      <c r="P20">
+        <v>4.75</v>
+      </c>
+      <c r="Q20">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="R20">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="S20">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="T20">
+        <v>0.17399999999999899</v>
+      </c>
+      <c r="V20">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="W20">
+        <v>0.17</v>
+      </c>
+      <c r="AD20">
+        <v>6.8000000000000005E-4</v>
+      </c>
+      <c r="AK20">
+        <v>4</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>1</v>
+      </c>
+      <c r="AN20">
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>70</v>
+      </c>
+      <c r="AQ20">
+        <v>9</v>
+      </c>
+      <c r="AR20">
+        <v>16</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>3000</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
         <f>5.03*1000</f>
         <v>5030</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G21" s="3">
         <f>427.3*1000</f>
         <v>427300</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H21" s="3">
         <v>0.9</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
         <f>3.68*1000</f>
         <v>3680</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L21" s="3">
         <f>2.9*1000</f>
         <v>2900</v>
       </c>
-      <c r="M17" s="3">
+      <c r="M21" s="3">
         <v>0.81</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3">
+      <c r="N21" s="3"/>
+      <c r="O21" s="3">
         <f>2.1/1000</f>
         <v>2.1000000000000003E-3</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P21" s="3">
         <v>12.35</v>
       </c>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3">
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3">
         <v>1.2</v>
       </c>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3">
+      <c r="U21" s="3"/>
+      <c r="V21" s="3">
         <v>0.3</v>
       </c>
-      <c r="W17" s="3">
+      <c r="W21" s="3">
         <v>0.6</v>
       </c>
-      <c r="AK17" s="3">
+      <c r="AK21" s="3">
         <v>9</v>
       </c>
-      <c r="AL17" s="3"/>
-      <c r="AM17" s="3">
+      <c r="AL21" s="3"/>
+      <c r="AM21" s="3">
         <v>2</v>
       </c>
-      <c r="AP17" s="3">
+      <c r="AP21" s="3">
         <v>59</v>
       </c>
-      <c r="AQ17" s="3">
+      <c r="AQ21" s="3">
         <v>13</v>
       </c>
-      <c r="AR17" s="3">
+      <c r="AR21" s="3">
         <v>17</v>
       </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>3001</v>
+      </c>
+      <c r="B22" s="3">
+        <v>42.490473000000001</v>
+      </c>
+      <c r="C22" s="3">
+        <v>43.224142999999899</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="3">
+        <v>470</v>
+      </c>
+      <c r="F22" s="3">
+        <v>7480</v>
+      </c>
+      <c r="G22" s="3">
+        <v>418700</v>
+      </c>
+      <c r="K22" s="3">
+        <v>9170</v>
+      </c>
+      <c r="L22" s="3">
+        <v>350</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="O22" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="P22" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="W22" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="AK22" s="3">
+        <v>9</v>
+      </c>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3">
+        <v>3</v>
+      </c>
+      <c r="AP22" s="3">
+        <v>61</v>
+      </c>
+      <c r="AQ22" s="3">
+        <v>9</v>
+      </c>
+      <c r="AR22" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
north valley is not so good for now
</commit_message>
<xml_diff>
--- a/North_Valley/data/North_Valley_Data.xlsx
+++ b/North_Valley/data/North_Valley_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -168,16 +168,13 @@
     <t>%</t>
   </si>
   <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>Left</t>
-  </si>
-  <si>
     <t>Mix</t>
   </si>
   <si>
     <t>Moraine</t>
+  </si>
+  <si>
+    <t>Sides</t>
   </si>
 </sst>
 </file>
@@ -528,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,7 +816,7 @@
         <v>43.226531999652138</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E3">
         <v>1020</v>
@@ -908,7 +905,7 @@
         <v>43.227588999832513</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -1003,7 +1000,7 @@
         <v>43.228735999666704</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>1070</v>
@@ -1098,7 +1095,7 @@
         <v>43.229299000448577</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <v>950</v>
@@ -1199,7 +1196,7 @@
         <v>43.229126999711298</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E7">
         <v>3260</v>
@@ -1291,7 +1288,7 @@
         <v>43.229760000123967</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>240</v>
@@ -1374,7 +1371,7 @@
         <v>43.230735000120212</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <v>4620</v>
@@ -1478,7 +1475,7 @@
         <v>43.231610000001517</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>14270</v>
@@ -1576,7 +1573,7 @@
         <v>43.232109999676823</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11">
         <v>83</v>
@@ -1665,7 +1662,7 @@
         <v>43.229892999962033</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E12">
         <v>370</v>
@@ -1748,7 +1745,7 @@
         <v>43.229155000103219</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>260</v>
@@ -1852,7 +1849,7 @@
         <v>43.228182000199183</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E14">
         <v>230</v>
@@ -1938,7 +1935,7 @@
         <v>43.228030000384251</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>4104</v>
@@ -2033,7 +2030,7 @@
         <v>43.229045000426481</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16">
         <v>20540</v>
@@ -2125,7 +2122,7 @@
         <v>43.229779999999998</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17">
         <v>125</v>
@@ -2235,7 +2232,7 @@
         <v>43.229580999963218</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18">
         <v>1030</v>
@@ -2336,7 +2333,7 @@
         <v>43.233797000131517</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E19">
         <v>1260</v>
@@ -2431,7 +2428,7 @@
         <v>43.227299262550957</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20">
         <v>50</v>
@@ -2516,7 +2513,7 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3">
@@ -2592,7 +2589,7 @@
         <v>43.224142999999899</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E22" s="3">
         <v>470</v>

</xml_diff>